<commit_message>
Updated xpaths for RecordDockeetingCallbackMessage
</commit_message>
<xml_diff>
--- a/shared/ojb-resources-common/src/main/resources/ssp/Docketing_Callback_Recording/artifacts/service_model/information_model/IEPD/documentation/RecordDocketingCallbackMessage.xlsx
+++ b/shared/ojb-resources-common/src/main/resources/ssp/Docketing_Callback_Recording/artifacts/service_model/information_model/IEPD/documentation/RecordDocketingCallbackMessage.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11440" uniqueCount="2038">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11470" uniqueCount="2041">
   <si>
     <t xml:space="preserve">   Line</t>
   </si>
@@ -6187,13 +6187,22 @@
     <t>Court Information</t>
   </si>
   <si>
-    <t>Person Information</t>
-  </si>
-  <si>
     <t>Bar Number</t>
   </si>
   <si>
-    <t>Jurisdiction</t>
+    <t>Case Filed Date</t>
+  </si>
+  <si>
+    <t>Judge Information</t>
+  </si>
+  <si>
+    <t>Sending MDE Profile Code</t>
+  </si>
+  <si>
+    <t>Sending MDE</t>
+  </si>
+  <si>
+    <t>Sending MDE Location Code</t>
   </si>
 </sst>
 </file>
@@ -6664,7 +6673,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="311">
+  <cellXfs count="315">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="8" fillId="10" borderId="5" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -7192,12 +7201,163 @@
     <xf numFmtId="1" fontId="6" fillId="0" borderId="5" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="27" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="27" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="27" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="27" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="27" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="23" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="23" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="23" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="23" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="22" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="22" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="22" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="22" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="13" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="11" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="19" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="19" borderId="2" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="20" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="20" borderId="2" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="17" fillId="21" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="21" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="21" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="21" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="18" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="18" borderId="2" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="15" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="15" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="2" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="16" borderId="2" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="2" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="3" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="4" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="13" borderId="2" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -7236,158 +7396,6 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="8" borderId="2" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="2" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="3" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="4" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="15" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="14" fillId="15" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="2" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="12" fillId="16" borderId="2" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="18" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="18" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="18" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="16" fillId="18" borderId="2" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="19" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="12" fillId="19" borderId="2" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="20" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="12" fillId="20" borderId="2" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="17" fillId="21" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="21" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="21" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="21" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="22" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="22" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="22" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="22" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="27" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="27" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="27" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="27" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="27" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="23" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="23" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="23" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="23" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="10" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" textRotation="90" wrapText="1"/>
@@ -7478,20 +7486,14 @@
     <xf numFmtId="0" fontId="8" fillId="8" borderId="5" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="5" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="29" borderId="2" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -7502,11 +7504,32 @@
     <xf numFmtId="0" fontId="9" fillId="29" borderId="4" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="30" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="16">
@@ -7824,228 +7847,299 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B29"/>
+  <dimension ref="A1:C28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.140625" customWidth="1"/>
-    <col min="2" max="2" width="56.140625" customWidth="1"/>
+    <col min="1" max="1" width="28.140625" style="312" customWidth="1"/>
+    <col min="2" max="2" width="56.140625" style="312" customWidth="1"/>
+    <col min="3" max="3" width="97.140625" style="312" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="312"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="47" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="312" t="s">
+        <v>2039</v>
+      </c>
+      <c r="B1" s="312" t="s">
+        <v>2038</v>
+      </c>
+      <c r="C1" s="46" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B2" s="312" t="s">
+        <v>2040</v>
+      </c>
+      <c r="C2" s="46" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="311" t="s">
         <v>2033</v>
       </c>
-      <c r="B1" s="47" t="str">
+      <c r="B3" s="314" t="str">
         <f>eFilingCriminalResponseElement!D6</f>
         <v>Uniform Offense Code (UOCT)</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="47"/>
-      <c r="B2" s="47" t="str">
+    <row r="4" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="311"/>
+      <c r="B4" s="311" t="str">
         <f>eFilingCriminalResponseElement!D12</f>
         <v>Charge Tracking Number</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="47"/>
-      <c r="B3" s="47" t="str">
-        <f>eFilingCriminalResponseElement!O3</f>
-        <v>Criminal Case Charge</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="47"/>
-      <c r="B4" t="str">
+      <c r="C4" s="46" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="311"/>
+      <c r="B5" s="312" t="str">
         <f>eFilingCriminalResponseElement!O4</f>
         <v>Charge Statute</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="47" t="s">
+      <c r="C5" s="46" t="s">
+        <v>779</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="311" t="s">
         <v>2034</v>
       </c>
-      <c r="B5" s="47" t="str">
+      <c r="B6" s="311" t="str">
         <f>'eFiling-CoreResponse'!AB46</f>
         <v>Court Office Code</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="47" t="s">
+      <c r="C6" s="46" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="311" t="s">
         <v>141</v>
       </c>
-      <c r="B6" s="47" t="str">
+      <c r="B7" s="311" t="str">
         <f>'eFiling-CoreResponse'!AB32</f>
         <v>Case Description</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="47"/>
-      <c r="B7" s="47" t="str">
+      <c r="C7" s="46" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="311"/>
+      <c r="B8" s="311" t="str">
         <f>'eFiling-CoreResponse'!AB33</f>
         <v>Case Title</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="47"/>
-      <c r="B8" s="47" t="str">
+      <c r="C8" s="46" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="311"/>
+      <c r="B9" s="311" t="str">
         <f>'eFiling-CoreResponse'!AB34</f>
         <v>Case Type Code</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="47"/>
-      <c r="B9" s="47" t="str">
+      <c r="C9" s="46" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="311"/>
+      <c r="B10" s="311" t="str">
         <f>'eFiling-CoreResponse'!AB35</f>
         <v>Case Number</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="47" t="s">
+      <c r="C10" s="46" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="311"/>
+      <c r="B11" s="311" t="s">
+        <v>2036</v>
+      </c>
+      <c r="C11" s="47" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="311" t="s">
         <v>2031</v>
       </c>
-      <c r="B10" s="47" t="str">
+      <c r="B12" s="311" t="str">
         <f>'eFiling-CoreResponse'!AB48</f>
         <v>Event Code Description</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="47"/>
-      <c r="B11" s="47" t="str">
+      <c r="C12" s="46" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="311"/>
+      <c r="B13" s="311" t="str">
         <f>'eFiling-CoreResponse'!AB49</f>
         <v>CourtEventEnteredOnDocketDate</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="47"/>
-      <c r="B12" s="47" t="str">
+      <c r="C13" s="46" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="311"/>
+      <c r="B14" s="311" t="str">
         <f>'eFiling-CoreResponse'!AB50</f>
         <v xml:space="preserve">Event Code </v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="47"/>
-      <c r="B13" s="47" t="str">
+      <c r="C14" s="46" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="311"/>
+      <c r="B15" s="311" t="str">
         <f>'eFiling-CoreResponse'!AB51</f>
         <v>Event Location Code</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="47"/>
-      <c r="B14" s="47" t="str">
-        <f>'eFiling-CoreResponse'!AB59</f>
-        <v>Event Date</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="47"/>
-      <c r="B15" s="47" t="str">
+      <c r="C15" s="46" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="311"/>
+      <c r="B16" s="311" t="s">
+        <v>296</v>
+      </c>
+      <c r="C16" s="46" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="311"/>
+      <c r="B17" s="311" t="str">
         <f>'eFiling-CoreResponse'!AB57</f>
         <v>Event Start Time</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="47"/>
-      <c r="B16" s="47" t="str">
+      <c r="C17" s="46" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="311"/>
+      <c r="B18" s="311" t="str">
         <f>'eFiling-CoreResponse'!AB56</f>
         <v>Event End Time</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="47"/>
-      <c r="B17" s="47" t="str">
+      <c r="C18" s="46" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="311"/>
+      <c r="B19" s="311" t="str">
         <f>'eFiling-CoreResponse'!AB53</f>
         <v>CourtEventJudge</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="47" t="s">
+      <c r="C19" s="46" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="311" t="s">
         <v>2032</v>
       </c>
-      <c r="B18" s="193" t="str">
+      <c r="B20" s="313" t="str">
         <f>CoreDefendantPtyFilingResponse!D6</f>
         <v>Defendant Party Person</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="47"/>
-      <c r="B19" s="47" t="str">
+      <c r="C20" s="46" t="s">
+        <v>828</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A21" s="311"/>
+      <c r="B21" s="311" t="str">
         <f>CoreDefendantAttyFilingResponse!AA3</f>
         <v>Case Defense (Defendant) Attorney</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="47"/>
-      <c r="B20" s="193" t="str">
-        <f>CoreInitiatingPtyFilingResponse!Z6</f>
-        <v>Plaintiff Party Person</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="47"/>
-      <c r="B21" s="47" t="str">
+      <c r="C21" s="36" t="s">
+        <v>1290</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" s="311"/>
+      <c r="B22" s="311" t="str">
         <f>CoreInitiatingAttyResponse!N3</f>
         <v>Case Initiating (Plaintiff) Attorney</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="47"/>
-      <c r="B22" s="47" t="str">
-        <f>CoreParticipantPtyFilingRespons!N3</f>
-        <v>Participants (Miscellaneous Party Organization Information)</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="47" t="s">
+      <c r="C22" s="22" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="311" t="s">
         <v>2030</v>
       </c>
-      <c r="B23" s="47" t="str">
+      <c r="B23" s="311" t="str">
         <f>'eFiling-CoreResponse'!AB25</f>
         <v>ErrorCode</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="47"/>
-      <c r="B24" s="47" t="str">
+      <c r="C23" s="310" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="311"/>
+      <c r="B24" s="311" t="str">
         <f>'eFiling-CoreResponse'!AB26</f>
         <v>ErrorText</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="47"/>
-      <c r="B25" s="47" t="str">
+      <c r="C24" s="310" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="311"/>
+      <c r="B25" s="311" t="str">
         <f>'eFiling-CoreResponse'!AB27</f>
         <v>FilingStatusCode</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="47" t="s">
+      <c r="C25" s="52" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A26" s="311" t="s">
+        <v>2037</v>
+      </c>
+      <c r="B26" s="311" t="s">
+        <v>8</v>
+      </c>
+      <c r="C26" s="46" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A27" s="311"/>
+      <c r="B27" s="311" t="s">
         <v>2035</v>
       </c>
-      <c r="B26" s="47" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="47"/>
-      <c r="B27" s="47" t="s">
-        <v>2036</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="47"/>
-      <c r="B28" s="47" t="s">
-        <v>2037</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="47"/>
-      <c r="B29" s="47" t="str">
+      <c r="C27" s="67" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="311"/>
+      <c r="B28" s="314" t="str">
         <f>eFilingCriminalResponseElement!D9</f>
         <v>Arrest Tracking Number</v>
       </c>
@@ -8085,10 +8179,10 @@
   <dimension ref="A1:AV188"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="AL3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="2" topLeftCell="Z70" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D3" sqref="D3"/>
+      <selection pane="bottomRight" activeCell="AC54" sqref="AC54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8136,72 +8230,72 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:48" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="203" t="s">
+      <c r="A1" s="262" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="205" t="s">
+      <c r="B1" s="264" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="205" t="s">
+      <c r="C1" s="264" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="207" t="s">
+      <c r="D1" s="266" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="208"/>
-      <c r="F1" s="208"/>
-      <c r="G1" s="208"/>
-      <c r="H1" s="208"/>
-      <c r="I1" s="208"/>
-      <c r="J1" s="208"/>
-      <c r="K1" s="208"/>
-      <c r="L1" s="208"/>
-      <c r="M1" s="208"/>
-      <c r="N1" s="209"/>
-      <c r="O1" s="210" t="s">
+      <c r="E1" s="267"/>
+      <c r="F1" s="267"/>
+      <c r="G1" s="267"/>
+      <c r="H1" s="267"/>
+      <c r="I1" s="267"/>
+      <c r="J1" s="267"/>
+      <c r="K1" s="267"/>
+      <c r="L1" s="267"/>
+      <c r="M1" s="267"/>
+      <c r="N1" s="268"/>
+      <c r="O1" s="269" t="s">
         <v>4</v>
       </c>
-      <c r="P1" s="208"/>
-      <c r="Q1" s="208"/>
-      <c r="R1" s="208"/>
-      <c r="S1" s="208"/>
-      <c r="T1" s="208"/>
-      <c r="U1" s="208"/>
-      <c r="V1" s="208"/>
-      <c r="W1" s="208"/>
-      <c r="X1" s="208"/>
-      <c r="Y1" s="208"/>
-      <c r="Z1" s="209"/>
-      <c r="AA1" s="211" t="s">
+      <c r="P1" s="267"/>
+      <c r="Q1" s="267"/>
+      <c r="R1" s="267"/>
+      <c r="S1" s="267"/>
+      <c r="T1" s="267"/>
+      <c r="U1" s="267"/>
+      <c r="V1" s="267"/>
+      <c r="W1" s="267"/>
+      <c r="X1" s="267"/>
+      <c r="Y1" s="267"/>
+      <c r="Z1" s="268"/>
+      <c r="AA1" s="270" t="s">
         <v>5</v>
       </c>
-      <c r="AB1" s="208"/>
-      <c r="AC1" s="208"/>
-      <c r="AD1" s="208"/>
-      <c r="AE1" s="208"/>
-      <c r="AF1" s="208"/>
-      <c r="AG1" s="208"/>
-      <c r="AH1" s="208"/>
-      <c r="AI1" s="208"/>
-      <c r="AJ1" s="208"/>
-      <c r="AK1" s="209"/>
-      <c r="AL1" s="212" t="s">
+      <c r="AB1" s="267"/>
+      <c r="AC1" s="267"/>
+      <c r="AD1" s="267"/>
+      <c r="AE1" s="267"/>
+      <c r="AF1" s="267"/>
+      <c r="AG1" s="267"/>
+      <c r="AH1" s="267"/>
+      <c r="AI1" s="267"/>
+      <c r="AJ1" s="267"/>
+      <c r="AK1" s="268"/>
+      <c r="AL1" s="253" t="s">
         <v>6</v>
       </c>
-      <c r="AM1" s="213"/>
-      <c r="AN1" s="213"/>
-      <c r="AO1" s="213"/>
-      <c r="AP1" s="213"/>
-      <c r="AQ1" s="213"/>
-      <c r="AR1" s="214"/>
+      <c r="AM1" s="254"/>
+      <c r="AN1" s="254"/>
+      <c r="AO1" s="254"/>
+      <c r="AP1" s="254"/>
+      <c r="AQ1" s="254"/>
+      <c r="AR1" s="255"/>
       <c r="AS1" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:48" ht="60" x14ac:dyDescent="0.25">
-      <c r="A2" s="204"/>
-      <c r="B2" s="206"/>
-      <c r="C2" s="206"/>
+      <c r="A2" s="263"/>
+      <c r="B2" s="265"/>
+      <c r="C2" s="265"/>
       <c r="D2" s="2" t="s">
         <v>8</v>
       </c>
@@ -10353,55 +10447,55 @@
       </c>
       <c r="B28" s="9"/>
       <c r="C28" s="9"/>
-      <c r="D28" s="215" t="s">
+      <c r="D28" s="198" t="s">
         <v>141</v>
       </c>
-      <c r="E28" s="216"/>
-      <c r="F28" s="216"/>
-      <c r="G28" s="216"/>
-      <c r="H28" s="216"/>
-      <c r="I28" s="216"/>
-      <c r="J28" s="216"/>
-      <c r="K28" s="216"/>
-      <c r="L28" s="216"/>
-      <c r="M28" s="216"/>
-      <c r="N28" s="216"/>
-      <c r="O28" s="215" t="s">
+      <c r="E28" s="199"/>
+      <c r="F28" s="199"/>
+      <c r="G28" s="199"/>
+      <c r="H28" s="199"/>
+      <c r="I28" s="199"/>
+      <c r="J28" s="199"/>
+      <c r="K28" s="199"/>
+      <c r="L28" s="199"/>
+      <c r="M28" s="199"/>
+      <c r="N28" s="199"/>
+      <c r="O28" s="198" t="s">
         <v>141</v>
       </c>
-      <c r="P28" s="216"/>
-      <c r="Q28" s="216"/>
-      <c r="R28" s="216"/>
-      <c r="S28" s="216"/>
-      <c r="T28" s="216"/>
-      <c r="U28" s="216"/>
-      <c r="V28" s="216"/>
-      <c r="W28" s="216"/>
-      <c r="X28" s="216"/>
-      <c r="Y28" s="216"/>
-      <c r="Z28" s="216"/>
-      <c r="AA28" s="217" t="s">
+      <c r="P28" s="199"/>
+      <c r="Q28" s="199"/>
+      <c r="R28" s="199"/>
+      <c r="S28" s="199"/>
+      <c r="T28" s="199"/>
+      <c r="U28" s="199"/>
+      <c r="V28" s="199"/>
+      <c r="W28" s="199"/>
+      <c r="X28" s="199"/>
+      <c r="Y28" s="199"/>
+      <c r="Z28" s="199"/>
+      <c r="AA28" s="200" t="s">
         <v>141</v>
       </c>
-      <c r="AB28" s="218"/>
-      <c r="AC28" s="218"/>
-      <c r="AD28" s="218"/>
-      <c r="AE28" s="218"/>
-      <c r="AF28" s="218"/>
-      <c r="AG28" s="218"/>
-      <c r="AH28" s="218"/>
-      <c r="AI28" s="218"/>
-      <c r="AJ28" s="218"/>
-      <c r="AK28" s="219"/>
-      <c r="AL28" s="217" t="s">
+      <c r="AB28" s="201"/>
+      <c r="AC28" s="201"/>
+      <c r="AD28" s="201"/>
+      <c r="AE28" s="201"/>
+      <c r="AF28" s="201"/>
+      <c r="AG28" s="201"/>
+      <c r="AH28" s="201"/>
+      <c r="AI28" s="201"/>
+      <c r="AJ28" s="201"/>
+      <c r="AK28" s="202"/>
+      <c r="AL28" s="200" t="s">
         <v>141</v>
       </c>
-      <c r="AM28" s="218"/>
-      <c r="AN28" s="218"/>
-      <c r="AO28" s="218"/>
-      <c r="AP28" s="218"/>
-      <c r="AQ28" s="218"/>
-      <c r="AR28" s="219"/>
+      <c r="AM28" s="201"/>
+      <c r="AN28" s="201"/>
+      <c r="AO28" s="201"/>
+      <c r="AP28" s="201"/>
+      <c r="AQ28" s="201"/>
+      <c r="AR28" s="202"/>
       <c r="AS28" s="54"/>
     </row>
     <row r="29" spans="1:48" x14ac:dyDescent="0.25">
@@ -13081,42 +13175,42 @@
       </c>
       <c r="B60" s="9"/>
       <c r="C60" s="9"/>
-      <c r="D60" s="194" t="s">
+      <c r="D60" s="213" t="s">
         <v>301</v>
       </c>
-      <c r="E60" s="195"/>
-      <c r="F60" s="195"/>
-      <c r="G60" s="195"/>
-      <c r="H60" s="195"/>
-      <c r="I60" s="195"/>
-      <c r="J60" s="195"/>
-      <c r="K60" s="195"/>
-      <c r="L60" s="195"/>
-      <c r="M60" s="195"/>
-      <c r="N60" s="196"/>
-      <c r="O60" s="197"/>
-      <c r="P60" s="198"/>
-      <c r="Q60" s="198"/>
-      <c r="R60" s="198"/>
-      <c r="S60" s="198"/>
-      <c r="T60" s="198"/>
-      <c r="U60" s="198"/>
-      <c r="V60" s="198"/>
-      <c r="W60" s="198"/>
-      <c r="X60" s="198"/>
-      <c r="Y60" s="198"/>
-      <c r="Z60" s="199"/>
-      <c r="AA60" s="200"/>
-      <c r="AB60" s="201"/>
-      <c r="AC60" s="201"/>
-      <c r="AD60" s="201"/>
-      <c r="AE60" s="201"/>
-      <c r="AF60" s="201"/>
-      <c r="AG60" s="201"/>
-      <c r="AH60" s="201"/>
-      <c r="AI60" s="201"/>
-      <c r="AJ60" s="201"/>
-      <c r="AK60" s="202"/>
+      <c r="E60" s="214"/>
+      <c r="F60" s="214"/>
+      <c r="G60" s="214"/>
+      <c r="H60" s="214"/>
+      <c r="I60" s="214"/>
+      <c r="J60" s="214"/>
+      <c r="K60" s="214"/>
+      <c r="L60" s="214"/>
+      <c r="M60" s="214"/>
+      <c r="N60" s="215"/>
+      <c r="O60" s="256"/>
+      <c r="P60" s="257"/>
+      <c r="Q60" s="257"/>
+      <c r="R60" s="257"/>
+      <c r="S60" s="257"/>
+      <c r="T60" s="257"/>
+      <c r="U60" s="257"/>
+      <c r="V60" s="257"/>
+      <c r="W60" s="257"/>
+      <c r="X60" s="257"/>
+      <c r="Y60" s="257"/>
+      <c r="Z60" s="258"/>
+      <c r="AA60" s="259"/>
+      <c r="AB60" s="260"/>
+      <c r="AC60" s="260"/>
+      <c r="AD60" s="260"/>
+      <c r="AE60" s="260"/>
+      <c r="AF60" s="260"/>
+      <c r="AG60" s="260"/>
+      <c r="AH60" s="260"/>
+      <c r="AI60" s="260"/>
+      <c r="AJ60" s="260"/>
+      <c r="AK60" s="261"/>
       <c r="AL60" s="61"/>
       <c r="AM60" s="62"/>
       <c r="AN60" s="62"/>
@@ -13133,31 +13227,31 @@
       </c>
       <c r="B61" s="9"/>
       <c r="C61" s="9"/>
-      <c r="D61" s="220" t="s">
+      <c r="D61" s="244" t="s">
         <v>302</v>
       </c>
-      <c r="E61" s="221"/>
-      <c r="F61" s="221"/>
-      <c r="G61" s="221"/>
-      <c r="H61" s="221"/>
-      <c r="I61" s="221"/>
-      <c r="J61" s="221"/>
-      <c r="K61" s="221"/>
-      <c r="L61" s="221"/>
-      <c r="M61" s="221"/>
-      <c r="N61" s="222"/>
-      <c r="O61" s="223"/>
-      <c r="P61" s="221"/>
-      <c r="Q61" s="221"/>
-      <c r="R61" s="221"/>
-      <c r="S61" s="221"/>
-      <c r="T61" s="221"/>
-      <c r="U61" s="221"/>
-      <c r="V61" s="221"/>
-      <c r="W61" s="221"/>
-      <c r="X61" s="221"/>
-      <c r="Y61" s="221"/>
-      <c r="Z61" s="222"/>
+      <c r="E61" s="245"/>
+      <c r="F61" s="245"/>
+      <c r="G61" s="245"/>
+      <c r="H61" s="245"/>
+      <c r="I61" s="245"/>
+      <c r="J61" s="245"/>
+      <c r="K61" s="245"/>
+      <c r="L61" s="245"/>
+      <c r="M61" s="245"/>
+      <c r="N61" s="246"/>
+      <c r="O61" s="247"/>
+      <c r="P61" s="245"/>
+      <c r="Q61" s="245"/>
+      <c r="R61" s="245"/>
+      <c r="S61" s="245"/>
+      <c r="T61" s="245"/>
+      <c r="U61" s="245"/>
+      <c r="V61" s="245"/>
+      <c r="W61" s="245"/>
+      <c r="X61" s="245"/>
+      <c r="Y61" s="245"/>
+      <c r="Z61" s="246"/>
       <c r="AA61" s="64"/>
       <c r="AB61" s="62"/>
       <c r="AC61" s="62"/>
@@ -13185,31 +13279,31 @@
       </c>
       <c r="B62" s="9"/>
       <c r="C62" s="9"/>
-      <c r="D62" s="224" t="s">
+      <c r="D62" s="248" t="s">
         <v>303</v>
       </c>
-      <c r="E62" s="225"/>
-      <c r="F62" s="225"/>
-      <c r="G62" s="225"/>
-      <c r="H62" s="225"/>
-      <c r="I62" s="225"/>
-      <c r="J62" s="225"/>
-      <c r="K62" s="225"/>
-      <c r="L62" s="225"/>
-      <c r="M62" s="225"/>
-      <c r="N62" s="226"/>
-      <c r="O62" s="227"/>
-      <c r="P62" s="225"/>
-      <c r="Q62" s="225"/>
-      <c r="R62" s="225"/>
-      <c r="S62" s="225"/>
-      <c r="T62" s="225"/>
-      <c r="U62" s="225"/>
-      <c r="V62" s="225"/>
-      <c r="W62" s="225"/>
-      <c r="X62" s="225"/>
-      <c r="Y62" s="225"/>
-      <c r="Z62" s="226"/>
+      <c r="E62" s="249"/>
+      <c r="F62" s="249"/>
+      <c r="G62" s="249"/>
+      <c r="H62" s="249"/>
+      <c r="I62" s="249"/>
+      <c r="J62" s="249"/>
+      <c r="K62" s="249"/>
+      <c r="L62" s="249"/>
+      <c r="M62" s="249"/>
+      <c r="N62" s="250"/>
+      <c r="O62" s="251"/>
+      <c r="P62" s="249"/>
+      <c r="Q62" s="249"/>
+      <c r="R62" s="249"/>
+      <c r="S62" s="249"/>
+      <c r="T62" s="249"/>
+      <c r="U62" s="249"/>
+      <c r="V62" s="249"/>
+      <c r="W62" s="249"/>
+      <c r="X62" s="249"/>
+      <c r="Y62" s="249"/>
+      <c r="Z62" s="250"/>
       <c r="AA62" s="64"/>
       <c r="AB62" s="62"/>
       <c r="AC62" s="62"/>
@@ -13237,55 +13331,55 @@
       </c>
       <c r="B63" s="9"/>
       <c r="C63" s="9"/>
-      <c r="D63" s="228" t="s">
+      <c r="D63" s="252" t="s">
         <v>304</v>
       </c>
-      <c r="E63" s="216"/>
-      <c r="F63" s="216"/>
-      <c r="G63" s="216"/>
-      <c r="H63" s="216"/>
-      <c r="I63" s="216"/>
-      <c r="J63" s="216"/>
-      <c r="K63" s="216"/>
-      <c r="L63" s="216"/>
-      <c r="M63" s="216"/>
-      <c r="N63" s="216"/>
-      <c r="O63" s="228" t="s">
+      <c r="E63" s="199"/>
+      <c r="F63" s="199"/>
+      <c r="G63" s="199"/>
+      <c r="H63" s="199"/>
+      <c r="I63" s="199"/>
+      <c r="J63" s="199"/>
+      <c r="K63" s="199"/>
+      <c r="L63" s="199"/>
+      <c r="M63" s="199"/>
+      <c r="N63" s="199"/>
+      <c r="O63" s="252" t="s">
         <v>304</v>
       </c>
-      <c r="P63" s="216"/>
-      <c r="Q63" s="216"/>
-      <c r="R63" s="216"/>
-      <c r="S63" s="216"/>
-      <c r="T63" s="216"/>
-      <c r="U63" s="216"/>
-      <c r="V63" s="216"/>
-      <c r="W63" s="216"/>
-      <c r="X63" s="216"/>
-      <c r="Y63" s="216"/>
-      <c r="Z63" s="216"/>
-      <c r="AA63" s="229" t="s">
+      <c r="P63" s="199"/>
+      <c r="Q63" s="199"/>
+      <c r="R63" s="199"/>
+      <c r="S63" s="199"/>
+      <c r="T63" s="199"/>
+      <c r="U63" s="199"/>
+      <c r="V63" s="199"/>
+      <c r="W63" s="199"/>
+      <c r="X63" s="199"/>
+      <c r="Y63" s="199"/>
+      <c r="Z63" s="199"/>
+      <c r="AA63" s="237" t="s">
         <v>304</v>
       </c>
-      <c r="AB63" s="230"/>
-      <c r="AC63" s="230"/>
-      <c r="AD63" s="230"/>
-      <c r="AE63" s="230"/>
-      <c r="AF63" s="230"/>
-      <c r="AG63" s="230"/>
-      <c r="AH63" s="230"/>
-      <c r="AI63" s="230"/>
-      <c r="AJ63" s="230"/>
-      <c r="AK63" s="231"/>
-      <c r="AL63" s="229" t="s">
+      <c r="AB63" s="238"/>
+      <c r="AC63" s="238"/>
+      <c r="AD63" s="238"/>
+      <c r="AE63" s="238"/>
+      <c r="AF63" s="238"/>
+      <c r="AG63" s="238"/>
+      <c r="AH63" s="238"/>
+      <c r="AI63" s="238"/>
+      <c r="AJ63" s="238"/>
+      <c r="AK63" s="239"/>
+      <c r="AL63" s="237" t="s">
         <v>304</v>
       </c>
-      <c r="AM63" s="230"/>
-      <c r="AN63" s="230"/>
-      <c r="AO63" s="230"/>
-      <c r="AP63" s="230"/>
-      <c r="AQ63" s="230"/>
-      <c r="AR63" s="231"/>
+      <c r="AM63" s="238"/>
+      <c r="AN63" s="238"/>
+      <c r="AO63" s="238"/>
+      <c r="AP63" s="238"/>
+      <c r="AQ63" s="238"/>
+      <c r="AR63" s="239"/>
       <c r="AS63" s="66"/>
     </row>
     <row r="64" spans="1:45" ht="89.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -14881,55 +14975,55 @@
       </c>
       <c r="B83" s="9"/>
       <c r="C83" s="9"/>
-      <c r="D83" s="232" t="s">
+      <c r="D83" s="240" t="s">
         <v>385</v>
       </c>
-      <c r="E83" s="216"/>
-      <c r="F83" s="216"/>
-      <c r="G83" s="216"/>
-      <c r="H83" s="216"/>
-      <c r="I83" s="216"/>
-      <c r="J83" s="216"/>
-      <c r="K83" s="216"/>
-      <c r="L83" s="216"/>
-      <c r="M83" s="216"/>
-      <c r="N83" s="216"/>
-      <c r="O83" s="232" t="s">
+      <c r="E83" s="199"/>
+      <c r="F83" s="199"/>
+      <c r="G83" s="199"/>
+      <c r="H83" s="199"/>
+      <c r="I83" s="199"/>
+      <c r="J83" s="199"/>
+      <c r="K83" s="199"/>
+      <c r="L83" s="199"/>
+      <c r="M83" s="199"/>
+      <c r="N83" s="199"/>
+      <c r="O83" s="240" t="s">
         <v>385</v>
       </c>
-      <c r="P83" s="216"/>
-      <c r="Q83" s="216"/>
-      <c r="R83" s="216"/>
-      <c r="S83" s="216"/>
-      <c r="T83" s="216"/>
-      <c r="U83" s="216"/>
-      <c r="V83" s="216"/>
-      <c r="W83" s="216"/>
-      <c r="X83" s="216"/>
-      <c r="Y83" s="216"/>
-      <c r="Z83" s="216"/>
-      <c r="AA83" s="233" t="s">
+      <c r="P83" s="199"/>
+      <c r="Q83" s="199"/>
+      <c r="R83" s="199"/>
+      <c r="S83" s="199"/>
+      <c r="T83" s="199"/>
+      <c r="U83" s="199"/>
+      <c r="V83" s="199"/>
+      <c r="W83" s="199"/>
+      <c r="X83" s="199"/>
+      <c r="Y83" s="199"/>
+      <c r="Z83" s="199"/>
+      <c r="AA83" s="241" t="s">
         <v>385</v>
       </c>
-      <c r="AB83" s="234"/>
-      <c r="AC83" s="234"/>
-      <c r="AD83" s="234"/>
-      <c r="AE83" s="234"/>
-      <c r="AF83" s="234"/>
-      <c r="AG83" s="234"/>
-      <c r="AH83" s="234"/>
-      <c r="AI83" s="234"/>
-      <c r="AJ83" s="234"/>
-      <c r="AK83" s="235"/>
-      <c r="AL83" s="233" t="s">
+      <c r="AB83" s="242"/>
+      <c r="AC83" s="242"/>
+      <c r="AD83" s="242"/>
+      <c r="AE83" s="242"/>
+      <c r="AF83" s="242"/>
+      <c r="AG83" s="242"/>
+      <c r="AH83" s="242"/>
+      <c r="AI83" s="242"/>
+      <c r="AJ83" s="242"/>
+      <c r="AK83" s="243"/>
+      <c r="AL83" s="241" t="s">
         <v>385</v>
       </c>
-      <c r="AM83" s="234"/>
-      <c r="AN83" s="234"/>
-      <c r="AO83" s="234"/>
-      <c r="AP83" s="234"/>
-      <c r="AQ83" s="234"/>
-      <c r="AR83" s="235"/>
+      <c r="AM83" s="242"/>
+      <c r="AN83" s="242"/>
+      <c r="AO83" s="242"/>
+      <c r="AP83" s="242"/>
+      <c r="AQ83" s="242"/>
+      <c r="AR83" s="243"/>
       <c r="AS83" s="73"/>
     </row>
     <row r="84" spans="1:45" ht="26.25" x14ac:dyDescent="0.25">
@@ -15511,55 +15605,55 @@
       </c>
       <c r="B91" s="9"/>
       <c r="C91" s="9"/>
-      <c r="D91" s="215" t="s">
+      <c r="D91" s="198" t="s">
         <v>416</v>
       </c>
-      <c r="E91" s="216"/>
-      <c r="F91" s="216"/>
-      <c r="G91" s="216"/>
-      <c r="H91" s="216"/>
-      <c r="I91" s="216"/>
-      <c r="J91" s="216"/>
-      <c r="K91" s="216"/>
-      <c r="L91" s="216"/>
-      <c r="M91" s="216"/>
-      <c r="N91" s="216"/>
-      <c r="O91" s="215" t="s">
+      <c r="E91" s="199"/>
+      <c r="F91" s="199"/>
+      <c r="G91" s="199"/>
+      <c r="H91" s="199"/>
+      <c r="I91" s="199"/>
+      <c r="J91" s="199"/>
+      <c r="K91" s="199"/>
+      <c r="L91" s="199"/>
+      <c r="M91" s="199"/>
+      <c r="N91" s="199"/>
+      <c r="O91" s="198" t="s">
         <v>416</v>
       </c>
-      <c r="P91" s="216"/>
-      <c r="Q91" s="216"/>
-      <c r="R91" s="216"/>
-      <c r="S91" s="216"/>
-      <c r="T91" s="216"/>
-      <c r="U91" s="216"/>
-      <c r="V91" s="216"/>
-      <c r="W91" s="216"/>
-      <c r="X91" s="216"/>
-      <c r="Y91" s="216"/>
-      <c r="Z91" s="216"/>
-      <c r="AA91" s="217" t="s">
+      <c r="P91" s="199"/>
+      <c r="Q91" s="199"/>
+      <c r="R91" s="199"/>
+      <c r="S91" s="199"/>
+      <c r="T91" s="199"/>
+      <c r="U91" s="199"/>
+      <c r="V91" s="199"/>
+      <c r="W91" s="199"/>
+      <c r="X91" s="199"/>
+      <c r="Y91" s="199"/>
+      <c r="Z91" s="199"/>
+      <c r="AA91" s="200" t="s">
         <v>416</v>
       </c>
-      <c r="AB91" s="218"/>
-      <c r="AC91" s="218"/>
-      <c r="AD91" s="218"/>
-      <c r="AE91" s="218"/>
-      <c r="AF91" s="218"/>
-      <c r="AG91" s="218"/>
-      <c r="AH91" s="218"/>
-      <c r="AI91" s="218"/>
-      <c r="AJ91" s="218"/>
-      <c r="AK91" s="219"/>
-      <c r="AL91" s="217" t="s">
+      <c r="AB91" s="201"/>
+      <c r="AC91" s="201"/>
+      <c r="AD91" s="201"/>
+      <c r="AE91" s="201"/>
+      <c r="AF91" s="201"/>
+      <c r="AG91" s="201"/>
+      <c r="AH91" s="201"/>
+      <c r="AI91" s="201"/>
+      <c r="AJ91" s="201"/>
+      <c r="AK91" s="202"/>
+      <c r="AL91" s="200" t="s">
         <v>416</v>
       </c>
-      <c r="AM91" s="218"/>
-      <c r="AN91" s="218"/>
-      <c r="AO91" s="218"/>
-      <c r="AP91" s="218"/>
-      <c r="AQ91" s="218"/>
-      <c r="AR91" s="219"/>
+      <c r="AM91" s="201"/>
+      <c r="AN91" s="201"/>
+      <c r="AO91" s="201"/>
+      <c r="AP91" s="201"/>
+      <c r="AQ91" s="201"/>
+      <c r="AR91" s="202"/>
       <c r="AS91" s="79"/>
     </row>
     <row r="92" spans="1:45" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -15641,31 +15735,31 @@
       </c>
       <c r="B93" s="9"/>
       <c r="C93" s="9"/>
-      <c r="D93" s="236" t="s">
+      <c r="D93" s="233" t="s">
         <v>418</v>
       </c>
-      <c r="E93" s="237"/>
-      <c r="F93" s="237"/>
-      <c r="G93" s="237"/>
-      <c r="H93" s="237"/>
-      <c r="I93" s="237"/>
-      <c r="J93" s="237"/>
-      <c r="K93" s="237"/>
-      <c r="L93" s="237"/>
-      <c r="M93" s="237"/>
-      <c r="N93" s="238"/>
-      <c r="O93" s="239"/>
-      <c r="P93" s="237"/>
-      <c r="Q93" s="237"/>
-      <c r="R93" s="237"/>
-      <c r="S93" s="237"/>
-      <c r="T93" s="237"/>
-      <c r="U93" s="237"/>
-      <c r="V93" s="237"/>
-      <c r="W93" s="237"/>
-      <c r="X93" s="237"/>
-      <c r="Y93" s="237"/>
-      <c r="Z93" s="238"/>
+      <c r="E93" s="234"/>
+      <c r="F93" s="234"/>
+      <c r="G93" s="234"/>
+      <c r="H93" s="234"/>
+      <c r="I93" s="234"/>
+      <c r="J93" s="234"/>
+      <c r="K93" s="234"/>
+      <c r="L93" s="234"/>
+      <c r="M93" s="234"/>
+      <c r="N93" s="235"/>
+      <c r="O93" s="236"/>
+      <c r="P93" s="234"/>
+      <c r="Q93" s="234"/>
+      <c r="R93" s="234"/>
+      <c r="S93" s="234"/>
+      <c r="T93" s="234"/>
+      <c r="U93" s="234"/>
+      <c r="V93" s="234"/>
+      <c r="W93" s="234"/>
+      <c r="X93" s="234"/>
+      <c r="Y93" s="234"/>
+      <c r="Z93" s="235"/>
       <c r="AA93" s="64"/>
       <c r="AB93" s="62"/>
       <c r="AC93" s="62"/>
@@ -15693,31 +15787,31 @@
       </c>
       <c r="B94" s="9"/>
       <c r="C94" s="9"/>
-      <c r="D94" s="240" t="s">
+      <c r="D94" s="216" t="s">
         <v>419</v>
       </c>
-      <c r="E94" s="241"/>
-      <c r="F94" s="241"/>
-      <c r="G94" s="241"/>
-      <c r="H94" s="241"/>
-      <c r="I94" s="241"/>
-      <c r="J94" s="241"/>
-      <c r="K94" s="241"/>
-      <c r="L94" s="241"/>
-      <c r="M94" s="241"/>
-      <c r="N94" s="242"/>
-      <c r="O94" s="243"/>
-      <c r="P94" s="244"/>
-      <c r="Q94" s="244"/>
-      <c r="R94" s="244"/>
-      <c r="S94" s="244"/>
-      <c r="T94" s="244"/>
-      <c r="U94" s="244"/>
-      <c r="V94" s="244"/>
-      <c r="W94" s="244"/>
-      <c r="X94" s="244"/>
-      <c r="Y94" s="244"/>
-      <c r="Z94" s="245"/>
+      <c r="E94" s="217"/>
+      <c r="F94" s="217"/>
+      <c r="G94" s="217"/>
+      <c r="H94" s="217"/>
+      <c r="I94" s="217"/>
+      <c r="J94" s="217"/>
+      <c r="K94" s="217"/>
+      <c r="L94" s="217"/>
+      <c r="M94" s="217"/>
+      <c r="N94" s="218"/>
+      <c r="O94" s="219"/>
+      <c r="P94" s="220"/>
+      <c r="Q94" s="220"/>
+      <c r="R94" s="220"/>
+      <c r="S94" s="220"/>
+      <c r="T94" s="220"/>
+      <c r="U94" s="220"/>
+      <c r="V94" s="220"/>
+      <c r="W94" s="220"/>
+      <c r="X94" s="220"/>
+      <c r="Y94" s="220"/>
+      <c r="Z94" s="221"/>
       <c r="AA94" s="64"/>
       <c r="AB94" s="62"/>
       <c r="AC94" s="62"/>
@@ -15745,31 +15839,31 @@
       </c>
       <c r="B95" s="9"/>
       <c r="C95" s="9"/>
-      <c r="D95" s="246" t="s">
+      <c r="D95" s="222" t="s">
         <v>420</v>
       </c>
-      <c r="E95" s="247"/>
-      <c r="F95" s="247"/>
-      <c r="G95" s="247"/>
-      <c r="H95" s="247"/>
-      <c r="I95" s="247"/>
-      <c r="J95" s="247"/>
-      <c r="K95" s="247"/>
-      <c r="L95" s="247"/>
-      <c r="M95" s="247"/>
-      <c r="N95" s="248"/>
-      <c r="O95" s="249"/>
-      <c r="P95" s="250"/>
-      <c r="Q95" s="250"/>
-      <c r="R95" s="250"/>
-      <c r="S95" s="250"/>
-      <c r="T95" s="250"/>
-      <c r="U95" s="250"/>
-      <c r="V95" s="250"/>
-      <c r="W95" s="250"/>
-      <c r="X95" s="250"/>
-      <c r="Y95" s="250"/>
-      <c r="Z95" s="251"/>
+      <c r="E95" s="223"/>
+      <c r="F95" s="223"/>
+      <c r="G95" s="223"/>
+      <c r="H95" s="223"/>
+      <c r="I95" s="223"/>
+      <c r="J95" s="223"/>
+      <c r="K95" s="223"/>
+      <c r="L95" s="223"/>
+      <c r="M95" s="223"/>
+      <c r="N95" s="224"/>
+      <c r="O95" s="225"/>
+      <c r="P95" s="226"/>
+      <c r="Q95" s="226"/>
+      <c r="R95" s="226"/>
+      <c r="S95" s="226"/>
+      <c r="T95" s="226"/>
+      <c r="U95" s="226"/>
+      <c r="V95" s="226"/>
+      <c r="W95" s="226"/>
+      <c r="X95" s="226"/>
+      <c r="Y95" s="226"/>
+      <c r="Z95" s="227"/>
       <c r="AA95" s="64"/>
       <c r="AB95" s="62"/>
       <c r="AC95" s="62"/>
@@ -15797,42 +15891,42 @@
       </c>
       <c r="B96" s="9"/>
       <c r="C96" s="9"/>
-      <c r="D96" s="252" t="s">
+      <c r="D96" s="228" t="s">
         <v>421</v>
       </c>
-      <c r="E96" s="253"/>
-      <c r="F96" s="253"/>
-      <c r="G96" s="253"/>
-      <c r="H96" s="253"/>
-      <c r="I96" s="253"/>
-      <c r="J96" s="253"/>
-      <c r="K96" s="253"/>
-      <c r="L96" s="253"/>
-      <c r="M96" s="253"/>
-      <c r="N96" s="254"/>
-      <c r="O96" s="255"/>
-      <c r="P96" s="256"/>
-      <c r="Q96" s="256"/>
-      <c r="R96" s="256"/>
-      <c r="S96" s="256"/>
-      <c r="T96" s="256"/>
-      <c r="U96" s="256"/>
-      <c r="V96" s="256"/>
-      <c r="W96" s="256"/>
-      <c r="X96" s="256"/>
-      <c r="Y96" s="256"/>
-      <c r="Z96" s="256"/>
-      <c r="AA96" s="257"/>
-      <c r="AB96" s="257"/>
-      <c r="AC96" s="257"/>
-      <c r="AD96" s="257"/>
-      <c r="AE96" s="257"/>
-      <c r="AF96" s="257"/>
-      <c r="AG96" s="257"/>
-      <c r="AH96" s="257"/>
-      <c r="AI96" s="257"/>
-      <c r="AJ96" s="257"/>
-      <c r="AK96" s="258"/>
+      <c r="E96" s="229"/>
+      <c r="F96" s="229"/>
+      <c r="G96" s="229"/>
+      <c r="H96" s="229"/>
+      <c r="I96" s="229"/>
+      <c r="J96" s="229"/>
+      <c r="K96" s="229"/>
+      <c r="L96" s="229"/>
+      <c r="M96" s="229"/>
+      <c r="N96" s="230"/>
+      <c r="O96" s="231"/>
+      <c r="P96" s="232"/>
+      <c r="Q96" s="232"/>
+      <c r="R96" s="232"/>
+      <c r="S96" s="232"/>
+      <c r="T96" s="232"/>
+      <c r="U96" s="232"/>
+      <c r="V96" s="232"/>
+      <c r="W96" s="232"/>
+      <c r="X96" s="232"/>
+      <c r="Y96" s="232"/>
+      <c r="Z96" s="232"/>
+      <c r="AA96" s="207"/>
+      <c r="AB96" s="207"/>
+      <c r="AC96" s="207"/>
+      <c r="AD96" s="207"/>
+      <c r="AE96" s="207"/>
+      <c r="AF96" s="207"/>
+      <c r="AG96" s="207"/>
+      <c r="AH96" s="207"/>
+      <c r="AI96" s="207"/>
+      <c r="AJ96" s="207"/>
+      <c r="AK96" s="208"/>
       <c r="AL96" s="65"/>
       <c r="AM96" s="65"/>
       <c r="AN96" s="65"/>
@@ -15849,55 +15943,55 @@
       </c>
       <c r="B97" s="9"/>
       <c r="C97" s="9"/>
-      <c r="D97" s="259" t="s">
+      <c r="D97" s="209" t="s">
         <v>422</v>
       </c>
-      <c r="E97" s="216"/>
-      <c r="F97" s="216"/>
-      <c r="G97" s="216"/>
-      <c r="H97" s="216"/>
-      <c r="I97" s="216"/>
-      <c r="J97" s="216"/>
-      <c r="K97" s="216"/>
-      <c r="L97" s="216"/>
-      <c r="M97" s="216"/>
-      <c r="N97" s="216"/>
-      <c r="O97" s="259" t="s">
+      <c r="E97" s="199"/>
+      <c r="F97" s="199"/>
+      <c r="G97" s="199"/>
+      <c r="H97" s="199"/>
+      <c r="I97" s="199"/>
+      <c r="J97" s="199"/>
+      <c r="K97" s="199"/>
+      <c r="L97" s="199"/>
+      <c r="M97" s="199"/>
+      <c r="N97" s="199"/>
+      <c r="O97" s="209" t="s">
         <v>422</v>
       </c>
-      <c r="P97" s="216"/>
-      <c r="Q97" s="216"/>
-      <c r="R97" s="216"/>
-      <c r="S97" s="216"/>
-      <c r="T97" s="216"/>
-      <c r="U97" s="216"/>
-      <c r="V97" s="216"/>
-      <c r="W97" s="216"/>
-      <c r="X97" s="216"/>
-      <c r="Y97" s="216"/>
-      <c r="Z97" s="216"/>
-      <c r="AA97" s="260" t="s">
+      <c r="P97" s="199"/>
+      <c r="Q97" s="199"/>
+      <c r="R97" s="199"/>
+      <c r="S97" s="199"/>
+      <c r="T97" s="199"/>
+      <c r="U97" s="199"/>
+      <c r="V97" s="199"/>
+      <c r="W97" s="199"/>
+      <c r="X97" s="199"/>
+      <c r="Y97" s="199"/>
+      <c r="Z97" s="199"/>
+      <c r="AA97" s="210" t="s">
         <v>422</v>
       </c>
-      <c r="AB97" s="261"/>
-      <c r="AC97" s="261"/>
-      <c r="AD97" s="261"/>
-      <c r="AE97" s="261"/>
-      <c r="AF97" s="261"/>
-      <c r="AG97" s="261"/>
-      <c r="AH97" s="261"/>
-      <c r="AI97" s="261"/>
-      <c r="AJ97" s="261"/>
-      <c r="AK97" s="262"/>
-      <c r="AL97" s="260" t="s">
+      <c r="AB97" s="211"/>
+      <c r="AC97" s="211"/>
+      <c r="AD97" s="211"/>
+      <c r="AE97" s="211"/>
+      <c r="AF97" s="211"/>
+      <c r="AG97" s="211"/>
+      <c r="AH97" s="211"/>
+      <c r="AI97" s="211"/>
+      <c r="AJ97" s="211"/>
+      <c r="AK97" s="212"/>
+      <c r="AL97" s="210" t="s">
         <v>422</v>
       </c>
-      <c r="AM97" s="261"/>
-      <c r="AN97" s="261"/>
-      <c r="AO97" s="261"/>
-      <c r="AP97" s="261"/>
-      <c r="AQ97" s="261"/>
-      <c r="AR97" s="262"/>
+      <c r="AM97" s="211"/>
+      <c r="AN97" s="211"/>
+      <c r="AO97" s="211"/>
+      <c r="AP97" s="211"/>
+      <c r="AQ97" s="211"/>
+      <c r="AR97" s="212"/>
       <c r="AS97" s="80"/>
     </row>
     <row r="98" spans="1:45" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -17287,30 +17381,30 @@
       </c>
       <c r="B114" s="9"/>
       <c r="C114" s="9"/>
-      <c r="D114" s="194" t="s">
+      <c r="D114" s="213" t="s">
         <v>470</v>
       </c>
-      <c r="E114" s="195"/>
-      <c r="F114" s="195"/>
-      <c r="G114" s="195"/>
-      <c r="H114" s="195"/>
-      <c r="I114" s="195"/>
-      <c r="J114" s="195"/>
-      <c r="K114" s="195"/>
-      <c r="L114" s="195"/>
-      <c r="M114" s="195"/>
-      <c r="N114" s="196"/>
-      <c r="O114" s="194"/>
-      <c r="P114" s="195"/>
-      <c r="Q114" s="195"/>
-      <c r="R114" s="195"/>
-      <c r="S114" s="195"/>
-      <c r="T114" s="195"/>
-      <c r="U114" s="195"/>
-      <c r="V114" s="195"/>
-      <c r="W114" s="195"/>
-      <c r="X114" s="195"/>
-      <c r="Y114" s="196"/>
+      <c r="E114" s="214"/>
+      <c r="F114" s="214"/>
+      <c r="G114" s="214"/>
+      <c r="H114" s="214"/>
+      <c r="I114" s="214"/>
+      <c r="J114" s="214"/>
+      <c r="K114" s="214"/>
+      <c r="L114" s="214"/>
+      <c r="M114" s="214"/>
+      <c r="N114" s="215"/>
+      <c r="O114" s="213"/>
+      <c r="P114" s="214"/>
+      <c r="Q114" s="214"/>
+      <c r="R114" s="214"/>
+      <c r="S114" s="214"/>
+      <c r="T114" s="214"/>
+      <c r="U114" s="214"/>
+      <c r="V114" s="214"/>
+      <c r="W114" s="214"/>
+      <c r="X114" s="214"/>
+      <c r="Y114" s="215"/>
       <c r="Z114" s="82"/>
       <c r="AA114" s="82"/>
       <c r="AB114" s="82"/>
@@ -17339,55 +17433,55 @@
       </c>
       <c r="B115" s="9"/>
       <c r="C115" s="9"/>
-      <c r="D115" s="215" t="s">
+      <c r="D115" s="198" t="s">
         <v>471</v>
       </c>
-      <c r="E115" s="216"/>
-      <c r="F115" s="216"/>
-      <c r="G115" s="216"/>
-      <c r="H115" s="216"/>
-      <c r="I115" s="216"/>
-      <c r="J115" s="216"/>
-      <c r="K115" s="216"/>
-      <c r="L115" s="216"/>
-      <c r="M115" s="216"/>
-      <c r="N115" s="216"/>
-      <c r="O115" s="215" t="s">
+      <c r="E115" s="199"/>
+      <c r="F115" s="199"/>
+      <c r="G115" s="199"/>
+      <c r="H115" s="199"/>
+      <c r="I115" s="199"/>
+      <c r="J115" s="199"/>
+      <c r="K115" s="199"/>
+      <c r="L115" s="199"/>
+      <c r="M115" s="199"/>
+      <c r="N115" s="199"/>
+      <c r="O115" s="198" t="s">
         <v>471</v>
       </c>
-      <c r="P115" s="216"/>
-      <c r="Q115" s="216"/>
-      <c r="R115" s="216"/>
-      <c r="S115" s="216"/>
-      <c r="T115" s="216"/>
-      <c r="U115" s="216"/>
-      <c r="V115" s="216"/>
-      <c r="W115" s="216"/>
-      <c r="X115" s="216"/>
-      <c r="Y115" s="216"/>
-      <c r="Z115" s="216"/>
-      <c r="AA115" s="217" t="s">
+      <c r="P115" s="199"/>
+      <c r="Q115" s="199"/>
+      <c r="R115" s="199"/>
+      <c r="S115" s="199"/>
+      <c r="T115" s="199"/>
+      <c r="U115" s="199"/>
+      <c r="V115" s="199"/>
+      <c r="W115" s="199"/>
+      <c r="X115" s="199"/>
+      <c r="Y115" s="199"/>
+      <c r="Z115" s="199"/>
+      <c r="AA115" s="200" t="s">
         <v>471</v>
       </c>
-      <c r="AB115" s="218"/>
-      <c r="AC115" s="218"/>
-      <c r="AD115" s="218"/>
-      <c r="AE115" s="218"/>
-      <c r="AF115" s="218"/>
-      <c r="AG115" s="218"/>
-      <c r="AH115" s="218"/>
-      <c r="AI115" s="218"/>
-      <c r="AJ115" s="218"/>
-      <c r="AK115" s="219"/>
-      <c r="AL115" s="217" t="s">
+      <c r="AB115" s="201"/>
+      <c r="AC115" s="201"/>
+      <c r="AD115" s="201"/>
+      <c r="AE115" s="201"/>
+      <c r="AF115" s="201"/>
+      <c r="AG115" s="201"/>
+      <c r="AH115" s="201"/>
+      <c r="AI115" s="201"/>
+      <c r="AJ115" s="201"/>
+      <c r="AK115" s="202"/>
+      <c r="AL115" s="200" t="s">
         <v>471</v>
       </c>
-      <c r="AM115" s="218"/>
-      <c r="AN115" s="218"/>
-      <c r="AO115" s="218"/>
-      <c r="AP115" s="218"/>
-      <c r="AQ115" s="218"/>
-      <c r="AR115" s="219"/>
+      <c r="AM115" s="201"/>
+      <c r="AN115" s="201"/>
+      <c r="AO115" s="201"/>
+      <c r="AP115" s="201"/>
+      <c r="AQ115" s="201"/>
+      <c r="AR115" s="202"/>
       <c r="AS115" s="79"/>
     </row>
     <row r="116" spans="1:45" ht="30" x14ac:dyDescent="0.25">
@@ -17589,55 +17683,55 @@
       <c r="C118" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="D118" s="268" t="s">
+      <c r="D118" s="203" t="s">
         <v>480</v>
       </c>
-      <c r="E118" s="216"/>
-      <c r="F118" s="216"/>
-      <c r="G118" s="216"/>
-      <c r="H118" s="216"/>
-      <c r="I118" s="216"/>
-      <c r="J118" s="216"/>
-      <c r="K118" s="216"/>
-      <c r="L118" s="216"/>
-      <c r="M118" s="216"/>
-      <c r="N118" s="216"/>
-      <c r="O118" s="268" t="s">
+      <c r="E118" s="199"/>
+      <c r="F118" s="199"/>
+      <c r="G118" s="199"/>
+      <c r="H118" s="199"/>
+      <c r="I118" s="199"/>
+      <c r="J118" s="199"/>
+      <c r="K118" s="199"/>
+      <c r="L118" s="199"/>
+      <c r="M118" s="199"/>
+      <c r="N118" s="199"/>
+      <c r="O118" s="203" t="s">
         <v>480</v>
       </c>
-      <c r="P118" s="216"/>
-      <c r="Q118" s="216"/>
-      <c r="R118" s="216"/>
-      <c r="S118" s="216"/>
-      <c r="T118" s="216"/>
-      <c r="U118" s="216"/>
-      <c r="V118" s="216"/>
-      <c r="W118" s="216"/>
-      <c r="X118" s="216"/>
-      <c r="Y118" s="216"/>
-      <c r="Z118" s="216"/>
-      <c r="AA118" s="269" t="s">
+      <c r="P118" s="199"/>
+      <c r="Q118" s="199"/>
+      <c r="R118" s="199"/>
+      <c r="S118" s="199"/>
+      <c r="T118" s="199"/>
+      <c r="U118" s="199"/>
+      <c r="V118" s="199"/>
+      <c r="W118" s="199"/>
+      <c r="X118" s="199"/>
+      <c r="Y118" s="199"/>
+      <c r="Z118" s="199"/>
+      <c r="AA118" s="204" t="s">
         <v>480</v>
       </c>
-      <c r="AB118" s="270"/>
-      <c r="AC118" s="270"/>
-      <c r="AD118" s="270"/>
-      <c r="AE118" s="270"/>
-      <c r="AF118" s="270"/>
-      <c r="AG118" s="270"/>
-      <c r="AH118" s="270"/>
-      <c r="AI118" s="270"/>
-      <c r="AJ118" s="270"/>
-      <c r="AK118" s="271"/>
-      <c r="AL118" s="269" t="s">
+      <c r="AB118" s="205"/>
+      <c r="AC118" s="205"/>
+      <c r="AD118" s="205"/>
+      <c r="AE118" s="205"/>
+      <c r="AF118" s="205"/>
+      <c r="AG118" s="205"/>
+      <c r="AH118" s="205"/>
+      <c r="AI118" s="205"/>
+      <c r="AJ118" s="205"/>
+      <c r="AK118" s="206"/>
+      <c r="AL118" s="204" t="s">
         <v>480</v>
       </c>
-      <c r="AM118" s="270"/>
-      <c r="AN118" s="270"/>
-      <c r="AO118" s="270"/>
-      <c r="AP118" s="270"/>
-      <c r="AQ118" s="270"/>
-      <c r="AR118" s="271"/>
+      <c r="AM118" s="205"/>
+      <c r="AN118" s="205"/>
+      <c r="AO118" s="205"/>
+      <c r="AP118" s="205"/>
+      <c r="AQ118" s="205"/>
+      <c r="AR118" s="206"/>
       <c r="AS118" s="84"/>
     </row>
     <row r="119" spans="1:45" ht="39" x14ac:dyDescent="0.25">
@@ -22713,55 +22807,55 @@
       </c>
       <c r="B179" s="9"/>
       <c r="C179" s="9"/>
-      <c r="D179" s="263" t="s">
+      <c r="D179" s="193" t="s">
         <v>747</v>
       </c>
-      <c r="E179" s="264"/>
-      <c r="F179" s="264"/>
-      <c r="G179" s="264"/>
-      <c r="H179" s="264"/>
-      <c r="I179" s="264"/>
-      <c r="J179" s="264"/>
-      <c r="K179" s="264"/>
-      <c r="L179" s="264"/>
-      <c r="M179" s="264"/>
-      <c r="N179" s="264"/>
-      <c r="O179" s="263" t="s">
+      <c r="E179" s="194"/>
+      <c r="F179" s="194"/>
+      <c r="G179" s="194"/>
+      <c r="H179" s="194"/>
+      <c r="I179" s="194"/>
+      <c r="J179" s="194"/>
+      <c r="K179" s="194"/>
+      <c r="L179" s="194"/>
+      <c r="M179" s="194"/>
+      <c r="N179" s="194"/>
+      <c r="O179" s="193" t="s">
         <v>747</v>
       </c>
-      <c r="P179" s="264"/>
-      <c r="Q179" s="264"/>
-      <c r="R179" s="264"/>
-      <c r="S179" s="264"/>
-      <c r="T179" s="264"/>
-      <c r="U179" s="264"/>
-      <c r="V179" s="264"/>
-      <c r="W179" s="264"/>
-      <c r="X179" s="264"/>
-      <c r="Y179" s="264"/>
-      <c r="Z179" s="264"/>
-      <c r="AA179" s="265" t="s">
+      <c r="P179" s="194"/>
+      <c r="Q179" s="194"/>
+      <c r="R179" s="194"/>
+      <c r="S179" s="194"/>
+      <c r="T179" s="194"/>
+      <c r="U179" s="194"/>
+      <c r="V179" s="194"/>
+      <c r="W179" s="194"/>
+      <c r="X179" s="194"/>
+      <c r="Y179" s="194"/>
+      <c r="Z179" s="194"/>
+      <c r="AA179" s="195" t="s">
         <v>747</v>
       </c>
-      <c r="AB179" s="266"/>
-      <c r="AC179" s="266"/>
-      <c r="AD179" s="266"/>
-      <c r="AE179" s="266"/>
-      <c r="AF179" s="266"/>
-      <c r="AG179" s="266"/>
-      <c r="AH179" s="266"/>
-      <c r="AI179" s="266"/>
-      <c r="AJ179" s="266"/>
-      <c r="AK179" s="267"/>
-      <c r="AL179" s="265" t="s">
+      <c r="AB179" s="196"/>
+      <c r="AC179" s="196"/>
+      <c r="AD179" s="196"/>
+      <c r="AE179" s="196"/>
+      <c r="AF179" s="196"/>
+      <c r="AG179" s="196"/>
+      <c r="AH179" s="196"/>
+      <c r="AI179" s="196"/>
+      <c r="AJ179" s="196"/>
+      <c r="AK179" s="197"/>
+      <c r="AL179" s="195" t="s">
         <v>747</v>
       </c>
-      <c r="AM179" s="266"/>
-      <c r="AN179" s="266"/>
-      <c r="AO179" s="266"/>
-      <c r="AP179" s="266"/>
-      <c r="AQ179" s="266"/>
-      <c r="AR179" s="267"/>
+      <c r="AM179" s="196"/>
+      <c r="AN179" s="196"/>
+      <c r="AO179" s="196"/>
+      <c r="AP179" s="196"/>
+      <c r="AQ179" s="196"/>
+      <c r="AR179" s="197"/>
       <c r="AS179" s="108"/>
     </row>
     <row r="180" spans="1:45" ht="26.25" x14ac:dyDescent="0.25">
@@ -23391,6 +23485,51 @@
   </sheetData>
   <autoFilter ref="A2:AS188"/>
   <mergeCells count="57">
+    <mergeCell ref="D60:N60"/>
+    <mergeCell ref="O60:Z60"/>
+    <mergeCell ref="AA60:AK60"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:N1"/>
+    <mergeCell ref="O1:Z1"/>
+    <mergeCell ref="AA1:AK1"/>
+    <mergeCell ref="AL1:AR1"/>
+    <mergeCell ref="D28:N28"/>
+    <mergeCell ref="O28:Z28"/>
+    <mergeCell ref="AA28:AK28"/>
+    <mergeCell ref="AL28:AR28"/>
+    <mergeCell ref="D61:N61"/>
+    <mergeCell ref="O61:Z61"/>
+    <mergeCell ref="D62:N62"/>
+    <mergeCell ref="O62:Z62"/>
+    <mergeCell ref="D63:N63"/>
+    <mergeCell ref="O63:Z63"/>
+    <mergeCell ref="AA63:AK63"/>
+    <mergeCell ref="AL63:AR63"/>
+    <mergeCell ref="D83:N83"/>
+    <mergeCell ref="O83:Z83"/>
+    <mergeCell ref="AA83:AK83"/>
+    <mergeCell ref="AL83:AR83"/>
+    <mergeCell ref="D91:N91"/>
+    <mergeCell ref="O91:Z91"/>
+    <mergeCell ref="AA91:AK91"/>
+    <mergeCell ref="AL91:AR91"/>
+    <mergeCell ref="D93:N93"/>
+    <mergeCell ref="O93:Z93"/>
+    <mergeCell ref="D114:N114"/>
+    <mergeCell ref="O114:Y114"/>
+    <mergeCell ref="D94:N94"/>
+    <mergeCell ref="O94:Z94"/>
+    <mergeCell ref="D95:N95"/>
+    <mergeCell ref="O95:Z95"/>
+    <mergeCell ref="D96:N96"/>
+    <mergeCell ref="O96:Z96"/>
+    <mergeCell ref="AA96:AK96"/>
+    <mergeCell ref="D97:N97"/>
+    <mergeCell ref="O97:Z97"/>
+    <mergeCell ref="AA97:AK97"/>
+    <mergeCell ref="AL97:AR97"/>
     <mergeCell ref="D179:N179"/>
     <mergeCell ref="O179:Z179"/>
     <mergeCell ref="AA179:AK179"/>
@@ -23403,51 +23542,6 @@
     <mergeCell ref="O118:Z118"/>
     <mergeCell ref="AA118:AK118"/>
     <mergeCell ref="AL118:AR118"/>
-    <mergeCell ref="AA96:AK96"/>
-    <mergeCell ref="D97:N97"/>
-    <mergeCell ref="O97:Z97"/>
-    <mergeCell ref="AA97:AK97"/>
-    <mergeCell ref="AL97:AR97"/>
-    <mergeCell ref="D114:N114"/>
-    <mergeCell ref="O114:Y114"/>
-    <mergeCell ref="D94:N94"/>
-    <mergeCell ref="O94:Z94"/>
-    <mergeCell ref="D95:N95"/>
-    <mergeCell ref="O95:Z95"/>
-    <mergeCell ref="D96:N96"/>
-    <mergeCell ref="O96:Z96"/>
-    <mergeCell ref="D91:N91"/>
-    <mergeCell ref="O91:Z91"/>
-    <mergeCell ref="AA91:AK91"/>
-    <mergeCell ref="AL91:AR91"/>
-    <mergeCell ref="D93:N93"/>
-    <mergeCell ref="O93:Z93"/>
-    <mergeCell ref="AA63:AK63"/>
-    <mergeCell ref="AL63:AR63"/>
-    <mergeCell ref="D83:N83"/>
-    <mergeCell ref="O83:Z83"/>
-    <mergeCell ref="AA83:AK83"/>
-    <mergeCell ref="AL83:AR83"/>
-    <mergeCell ref="D61:N61"/>
-    <mergeCell ref="O61:Z61"/>
-    <mergeCell ref="D62:N62"/>
-    <mergeCell ref="O62:Z62"/>
-    <mergeCell ref="D63:N63"/>
-    <mergeCell ref="O63:Z63"/>
-    <mergeCell ref="AL1:AR1"/>
-    <mergeCell ref="D28:N28"/>
-    <mergeCell ref="O28:Z28"/>
-    <mergeCell ref="AA28:AK28"/>
-    <mergeCell ref="AL28:AR28"/>
-    <mergeCell ref="D60:N60"/>
-    <mergeCell ref="O60:Z60"/>
-    <mergeCell ref="AA60:AK60"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:N1"/>
-    <mergeCell ref="O1:Z1"/>
-    <mergeCell ref="AA1:AK1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -23461,10 +23555,10 @@
   </sheetPr>
   <dimension ref="A1:AR32"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="O1" activePane="topRight" state="frozen"/>
       <selection activeCell="B23" sqref="B23"/>
-      <selection pane="topRight" activeCell="Q6" sqref="Q6"/>
+      <selection pane="topRight" activeCell="Q13" sqref="Q13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23515,71 +23609,71 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:44" s="116" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="272" t="s">
+      <c r="A1" s="271" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="205" t="s">
+      <c r="B1" s="264" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="205" t="s">
+      <c r="C1" s="264" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="207" t="s">
+      <c r="D1" s="266" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="274"/>
-      <c r="F1" s="274"/>
-      <c r="G1" s="274"/>
-      <c r="H1" s="274"/>
-      <c r="I1" s="274"/>
-      <c r="J1" s="274"/>
-      <c r="K1" s="274"/>
-      <c r="L1" s="274"/>
-      <c r="M1" s="274"/>
-      <c r="N1" s="275"/>
-      <c r="O1" s="210" t="s">
+      <c r="E1" s="273"/>
+      <c r="F1" s="273"/>
+      <c r="G1" s="273"/>
+      <c r="H1" s="273"/>
+      <c r="I1" s="273"/>
+      <c r="J1" s="273"/>
+      <c r="K1" s="273"/>
+      <c r="L1" s="273"/>
+      <c r="M1" s="273"/>
+      <c r="N1" s="274"/>
+      <c r="O1" s="269" t="s">
         <v>4</v>
       </c>
-      <c r="P1" s="276"/>
-      <c r="Q1" s="276"/>
-      <c r="R1" s="276"/>
-      <c r="S1" s="276"/>
-      <c r="T1" s="276"/>
-      <c r="U1" s="276"/>
-      <c r="V1" s="276"/>
-      <c r="W1" s="276"/>
-      <c r="X1" s="276"/>
-      <c r="Y1" s="276"/>
-      <c r="Z1" s="277"/>
-      <c r="AA1" s="211" t="s">
+      <c r="P1" s="275"/>
+      <c r="Q1" s="275"/>
+      <c r="R1" s="275"/>
+      <c r="S1" s="275"/>
+      <c r="T1" s="275"/>
+      <c r="U1" s="275"/>
+      <c r="V1" s="275"/>
+      <c r="W1" s="275"/>
+      <c r="X1" s="275"/>
+      <c r="Y1" s="275"/>
+      <c r="Z1" s="276"/>
+      <c r="AA1" s="270" t="s">
         <v>770</v>
       </c>
-      <c r="AB1" s="278"/>
-      <c r="AC1" s="278"/>
-      <c r="AD1" s="278"/>
-      <c r="AE1" s="278"/>
-      <c r="AF1" s="278"/>
-      <c r="AG1" s="278"/>
-      <c r="AH1" s="278"/>
-      <c r="AI1" s="278"/>
-      <c r="AJ1" s="279"/>
-      <c r="AK1" s="212" t="s">
+      <c r="AB1" s="277"/>
+      <c r="AC1" s="277"/>
+      <c r="AD1" s="277"/>
+      <c r="AE1" s="277"/>
+      <c r="AF1" s="277"/>
+      <c r="AG1" s="277"/>
+      <c r="AH1" s="277"/>
+      <c r="AI1" s="277"/>
+      <c r="AJ1" s="278"/>
+      <c r="AK1" s="253" t="s">
         <v>771</v>
       </c>
-      <c r="AL1" s="213"/>
-      <c r="AM1" s="213"/>
-      <c r="AN1" s="213"/>
-      <c r="AO1" s="213"/>
-      <c r="AP1" s="213"/>
-      <c r="AQ1" s="214"/>
+      <c r="AL1" s="254"/>
+      <c r="AM1" s="254"/>
+      <c r="AN1" s="254"/>
+      <c r="AO1" s="254"/>
+      <c r="AP1" s="254"/>
+      <c r="AQ1" s="255"/>
       <c r="AR1" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:44" s="116" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="273"/>
-      <c r="B2" s="206"/>
-      <c r="C2" s="206"/>
+      <c r="A2" s="272"/>
+      <c r="B2" s="265"/>
+      <c r="C2" s="265"/>
       <c r="D2" s="117" t="s">
         <v>8</v>
       </c>
@@ -24750,11 +24844,11 @@
   <dimension ref="A1:AS133"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="O3" activePane="bottomRight" state="frozen"/>
       <selection activeCell="B23" sqref="B23"/>
       <selection pane="topRight" activeCell="B23" sqref="B23"/>
       <selection pane="bottomLeft" activeCell="B23" sqref="B23"/>
-      <selection pane="bottomRight" activeCell="J115" sqref="J115"/>
+      <selection pane="bottomRight" activeCell="Q5" sqref="Q5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -24797,72 +24891,72 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:45" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="203" t="s">
+      <c r="A1" s="262" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="205" t="s">
+      <c r="B1" s="264" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="205" t="s">
+      <c r="C1" s="264" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="207" t="s">
+      <c r="D1" s="266" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="208"/>
-      <c r="F1" s="208"/>
-      <c r="G1" s="208"/>
-      <c r="H1" s="208"/>
-      <c r="I1" s="208"/>
-      <c r="J1" s="208"/>
-      <c r="K1" s="208"/>
-      <c r="L1" s="208"/>
-      <c r="M1" s="208"/>
-      <c r="N1" s="209"/>
-      <c r="O1" s="210" t="s">
+      <c r="E1" s="267"/>
+      <c r="F1" s="267"/>
+      <c r="G1" s="267"/>
+      <c r="H1" s="267"/>
+      <c r="I1" s="267"/>
+      <c r="J1" s="267"/>
+      <c r="K1" s="267"/>
+      <c r="L1" s="267"/>
+      <c r="M1" s="267"/>
+      <c r="N1" s="268"/>
+      <c r="O1" s="269" t="s">
         <v>4</v>
       </c>
-      <c r="P1" s="208"/>
-      <c r="Q1" s="208"/>
-      <c r="R1" s="208"/>
-      <c r="S1" s="208"/>
-      <c r="T1" s="208"/>
-      <c r="U1" s="208"/>
-      <c r="V1" s="208"/>
-      <c r="W1" s="208"/>
-      <c r="X1" s="208"/>
-      <c r="Y1" s="208"/>
-      <c r="Z1" s="209"/>
-      <c r="AA1" s="211" t="s">
+      <c r="P1" s="267"/>
+      <c r="Q1" s="267"/>
+      <c r="R1" s="267"/>
+      <c r="S1" s="267"/>
+      <c r="T1" s="267"/>
+      <c r="U1" s="267"/>
+      <c r="V1" s="267"/>
+      <c r="W1" s="267"/>
+      <c r="X1" s="267"/>
+      <c r="Y1" s="267"/>
+      <c r="Z1" s="268"/>
+      <c r="AA1" s="270" t="s">
         <v>5</v>
       </c>
-      <c r="AB1" s="208"/>
-      <c r="AC1" s="208"/>
-      <c r="AD1" s="208"/>
-      <c r="AE1" s="208"/>
-      <c r="AF1" s="208"/>
-      <c r="AG1" s="208"/>
-      <c r="AH1" s="208"/>
-      <c r="AI1" s="208"/>
-      <c r="AJ1" s="208"/>
-      <c r="AK1" s="209"/>
-      <c r="AL1" s="212" t="s">
+      <c r="AB1" s="267"/>
+      <c r="AC1" s="267"/>
+      <c r="AD1" s="267"/>
+      <c r="AE1" s="267"/>
+      <c r="AF1" s="267"/>
+      <c r="AG1" s="267"/>
+      <c r="AH1" s="267"/>
+      <c r="AI1" s="267"/>
+      <c r="AJ1" s="267"/>
+      <c r="AK1" s="268"/>
+      <c r="AL1" s="253" t="s">
         <v>6</v>
       </c>
-      <c r="AM1" s="213"/>
-      <c r="AN1" s="213"/>
-      <c r="AO1" s="213"/>
-      <c r="AP1" s="213"/>
-      <c r="AQ1" s="213"/>
-      <c r="AR1" s="214"/>
+      <c r="AM1" s="254"/>
+      <c r="AN1" s="254"/>
+      <c r="AO1" s="254"/>
+      <c r="AP1" s="254"/>
+      <c r="AQ1" s="254"/>
+      <c r="AR1" s="255"/>
       <c r="AS1" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:45" ht="60" x14ac:dyDescent="0.25">
-      <c r="A2" s="204"/>
-      <c r="B2" s="206"/>
-      <c r="C2" s="206"/>
+      <c r="A2" s="263"/>
+      <c r="B2" s="265"/>
+      <c r="C2" s="265"/>
       <c r="D2" s="2" t="s">
         <v>8</v>
       </c>
@@ -24997,53 +25091,53 @@
       </c>
       <c r="B3" s="133"/>
       <c r="C3" s="133"/>
-      <c r="D3" s="283" t="s">
+      <c r="D3" s="282" t="s">
         <v>820</v>
       </c>
-      <c r="E3" s="283"/>
-      <c r="F3" s="283"/>
-      <c r="G3" s="283"/>
-      <c r="H3" s="283"/>
-      <c r="I3" s="283"/>
-      <c r="J3" s="283"/>
-      <c r="K3" s="283"/>
-      <c r="L3" s="283"/>
-      <c r="M3" s="283"/>
-      <c r="N3" s="283"/>
-      <c r="O3" s="284" t="s">
+      <c r="E3" s="282"/>
+      <c r="F3" s="282"/>
+      <c r="G3" s="282"/>
+      <c r="H3" s="282"/>
+      <c r="I3" s="282"/>
+      <c r="J3" s="282"/>
+      <c r="K3" s="282"/>
+      <c r="L3" s="282"/>
+      <c r="M3" s="282"/>
+      <c r="N3" s="282"/>
+      <c r="O3" s="283" t="s">
         <v>821</v>
       </c>
-      <c r="P3" s="284"/>
-      <c r="Q3" s="284"/>
-      <c r="R3" s="284"/>
-      <c r="S3" s="284"/>
-      <c r="T3" s="284"/>
-      <c r="U3" s="284"/>
-      <c r="V3" s="284"/>
-      <c r="W3" s="284"/>
-      <c r="X3" s="284"/>
-      <c r="Y3" s="284"/>
+      <c r="P3" s="283"/>
+      <c r="Q3" s="283"/>
+      <c r="R3" s="283"/>
+      <c r="S3" s="283"/>
+      <c r="T3" s="283"/>
+      <c r="U3" s="283"/>
+      <c r="V3" s="283"/>
+      <c r="W3" s="283"/>
+      <c r="X3" s="283"/>
+      <c r="Y3" s="283"/>
       <c r="Z3" s="134"/>
-      <c r="AA3" s="283" t="s">
+      <c r="AA3" s="282" t="s">
         <v>821</v>
       </c>
-      <c r="AB3" s="283"/>
-      <c r="AC3" s="283"/>
-      <c r="AD3" s="283"/>
-      <c r="AE3" s="283"/>
-      <c r="AF3" s="283"/>
-      <c r="AG3" s="283"/>
-      <c r="AH3" s="283"/>
-      <c r="AI3" s="283"/>
-      <c r="AJ3" s="283"/>
-      <c r="AK3" s="285"/>
-      <c r="AL3" s="285"/>
-      <c r="AM3" s="286"/>
-      <c r="AN3" s="286"/>
-      <c r="AO3" s="286"/>
-      <c r="AP3" s="286"/>
-      <c r="AQ3" s="286"/>
-      <c r="AR3" s="286"/>
+      <c r="AB3" s="282"/>
+      <c r="AC3" s="282"/>
+      <c r="AD3" s="282"/>
+      <c r="AE3" s="282"/>
+      <c r="AF3" s="282"/>
+      <c r="AG3" s="282"/>
+      <c r="AH3" s="282"/>
+      <c r="AI3" s="282"/>
+      <c r="AJ3" s="282"/>
+      <c r="AK3" s="284"/>
+      <c r="AL3" s="284"/>
+      <c r="AM3" s="285"/>
+      <c r="AN3" s="285"/>
+      <c r="AO3" s="285"/>
+      <c r="AP3" s="285"/>
+      <c r="AQ3" s="285"/>
+      <c r="AR3" s="285"/>
       <c r="AS3" s="52"/>
     </row>
     <row r="4" spans="1:45" s="116" customFormat="1" ht="39" x14ac:dyDescent="0.25">
@@ -25203,53 +25297,53 @@
       </c>
       <c r="B6" s="133"/>
       <c r="C6" s="133"/>
-      <c r="D6" s="285" t="s">
+      <c r="D6" s="284" t="s">
         <v>835</v>
       </c>
-      <c r="E6" s="286"/>
-      <c r="F6" s="286"/>
-      <c r="G6" s="286"/>
-      <c r="H6" s="286"/>
-      <c r="I6" s="286"/>
-      <c r="J6" s="286"/>
-      <c r="K6" s="286"/>
-      <c r="L6" s="286"/>
-      <c r="M6" s="286"/>
-      <c r="N6" s="287"/>
-      <c r="O6" s="288" t="s">
+      <c r="E6" s="285"/>
+      <c r="F6" s="285"/>
+      <c r="G6" s="285"/>
+      <c r="H6" s="285"/>
+      <c r="I6" s="285"/>
+      <c r="J6" s="285"/>
+      <c r="K6" s="285"/>
+      <c r="L6" s="285"/>
+      <c r="M6" s="285"/>
+      <c r="N6" s="286"/>
+      <c r="O6" s="287" t="s">
         <v>835</v>
       </c>
-      <c r="P6" s="289"/>
-      <c r="Q6" s="289"/>
-      <c r="R6" s="289"/>
-      <c r="S6" s="289"/>
-      <c r="T6" s="289"/>
-      <c r="U6" s="289"/>
-      <c r="V6" s="289"/>
-      <c r="W6" s="289"/>
-      <c r="X6" s="289"/>
-      <c r="Y6" s="290"/>
+      <c r="P6" s="288"/>
+      <c r="Q6" s="288"/>
+      <c r="R6" s="288"/>
+      <c r="S6" s="288"/>
+      <c r="T6" s="288"/>
+      <c r="U6" s="288"/>
+      <c r="V6" s="288"/>
+      <c r="W6" s="288"/>
+      <c r="X6" s="288"/>
+      <c r="Y6" s="289"/>
       <c r="Z6" s="143"/>
-      <c r="AA6" s="285" t="s">
+      <c r="AA6" s="284" t="s">
         <v>835</v>
       </c>
-      <c r="AB6" s="286"/>
-      <c r="AC6" s="286"/>
-      <c r="AD6" s="286"/>
-      <c r="AE6" s="286"/>
-      <c r="AF6" s="286"/>
-      <c r="AG6" s="286"/>
-      <c r="AH6" s="286"/>
-      <c r="AI6" s="286"/>
-      <c r="AJ6" s="286"/>
-      <c r="AK6" s="286"/>
-      <c r="AL6" s="285"/>
-      <c r="AM6" s="286"/>
-      <c r="AN6" s="286"/>
-      <c r="AO6" s="286"/>
-      <c r="AP6" s="286"/>
-      <c r="AQ6" s="286"/>
-      <c r="AR6" s="286"/>
+      <c r="AB6" s="285"/>
+      <c r="AC6" s="285"/>
+      <c r="AD6" s="285"/>
+      <c r="AE6" s="285"/>
+      <c r="AF6" s="285"/>
+      <c r="AG6" s="285"/>
+      <c r="AH6" s="285"/>
+      <c r="AI6" s="285"/>
+      <c r="AJ6" s="285"/>
+      <c r="AK6" s="285"/>
+      <c r="AL6" s="284"/>
+      <c r="AM6" s="285"/>
+      <c r="AN6" s="285"/>
+      <c r="AO6" s="285"/>
+      <c r="AP6" s="285"/>
+      <c r="AQ6" s="285"/>
+      <c r="AR6" s="285"/>
       <c r="AS6" s="52"/>
     </row>
     <row r="7" spans="1:45" s="27" customFormat="1" ht="39" x14ac:dyDescent="0.25">
@@ -31599,53 +31693,53 @@
       </c>
       <c r="B80" s="133"/>
       <c r="C80" s="133"/>
-      <c r="D80" s="280" t="s">
+      <c r="D80" s="279" t="s">
         <v>1139</v>
       </c>
-      <c r="E80" s="281"/>
-      <c r="F80" s="281"/>
-      <c r="G80" s="281"/>
-      <c r="H80" s="281"/>
-      <c r="I80" s="281"/>
-      <c r="J80" s="281"/>
-      <c r="K80" s="281"/>
-      <c r="L80" s="281"/>
-      <c r="M80" s="281"/>
-      <c r="N80" s="282"/>
-      <c r="O80" s="280" t="s">
+      <c r="E80" s="280"/>
+      <c r="F80" s="280"/>
+      <c r="G80" s="280"/>
+      <c r="H80" s="280"/>
+      <c r="I80" s="280"/>
+      <c r="J80" s="280"/>
+      <c r="K80" s="280"/>
+      <c r="L80" s="280"/>
+      <c r="M80" s="280"/>
+      <c r="N80" s="281"/>
+      <c r="O80" s="279" t="s">
         <v>1139</v>
       </c>
-      <c r="P80" s="281"/>
-      <c r="Q80" s="281"/>
-      <c r="R80" s="281"/>
-      <c r="S80" s="281"/>
-      <c r="T80" s="281"/>
-      <c r="U80" s="281"/>
-      <c r="V80" s="281"/>
-      <c r="W80" s="281"/>
-      <c r="X80" s="281"/>
-      <c r="Y80" s="281"/>
-      <c r="Z80" s="282"/>
-      <c r="AA80" s="280" t="s">
+      <c r="P80" s="280"/>
+      <c r="Q80" s="280"/>
+      <c r="R80" s="280"/>
+      <c r="S80" s="280"/>
+      <c r="T80" s="280"/>
+      <c r="U80" s="280"/>
+      <c r="V80" s="280"/>
+      <c r="W80" s="280"/>
+      <c r="X80" s="280"/>
+      <c r="Y80" s="280"/>
+      <c r="Z80" s="281"/>
+      <c r="AA80" s="279" t="s">
         <v>1139</v>
       </c>
-      <c r="AB80" s="281"/>
-      <c r="AC80" s="281"/>
-      <c r="AD80" s="281"/>
-      <c r="AE80" s="281"/>
-      <c r="AF80" s="281"/>
-      <c r="AG80" s="281"/>
-      <c r="AH80" s="281"/>
-      <c r="AI80" s="281"/>
-      <c r="AJ80" s="281"/>
-      <c r="AK80" s="281"/>
-      <c r="AL80" s="280"/>
-      <c r="AM80" s="281"/>
-      <c r="AN80" s="281"/>
-      <c r="AO80" s="281"/>
-      <c r="AP80" s="281"/>
-      <c r="AQ80" s="281"/>
-      <c r="AR80" s="281"/>
+      <c r="AB80" s="280"/>
+      <c r="AC80" s="280"/>
+      <c r="AD80" s="280"/>
+      <c r="AE80" s="280"/>
+      <c r="AF80" s="280"/>
+      <c r="AG80" s="280"/>
+      <c r="AH80" s="280"/>
+      <c r="AI80" s="280"/>
+      <c r="AJ80" s="280"/>
+      <c r="AK80" s="280"/>
+      <c r="AL80" s="279"/>
+      <c r="AM80" s="280"/>
+      <c r="AN80" s="280"/>
+      <c r="AO80" s="280"/>
+      <c r="AP80" s="280"/>
+      <c r="AQ80" s="280"/>
+      <c r="AR80" s="280"/>
       <c r="AS80" s="150"/>
     </row>
     <row r="81" spans="1:45" s="27" customFormat="1" ht="39" x14ac:dyDescent="0.25">
@@ -36227,6 +36321,11 @@
   </sheetData>
   <autoFilter ref="A2:AS133"/>
   <mergeCells count="19">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:N1"/>
+    <mergeCell ref="O1:Z1"/>
     <mergeCell ref="D80:N80"/>
     <mergeCell ref="O80:Z80"/>
     <mergeCell ref="AA80:AK80"/>
@@ -36241,11 +36340,6 @@
     <mergeCell ref="AA6:AK6"/>
     <mergeCell ref="AL6:AR6"/>
     <mergeCell ref="AA1:AK1"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:N1"/>
-    <mergeCell ref="O1:Z1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -36259,7 +36353,7 @@
   <dimension ref="A1:AS51"/>
   <sheetViews>
     <sheetView topLeftCell="T1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AC24" sqref="AC24"/>
+      <selection activeCell="AC6" sqref="AC6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -36301,72 +36395,72 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:45" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="295" t="s">
+      <c r="A1" s="294" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="205" t="s">
+      <c r="B1" s="264" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="205" t="s">
+      <c r="C1" s="264" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="297" t="s">
+      <c r="D1" s="296" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="298"/>
-      <c r="F1" s="298"/>
-      <c r="G1" s="298"/>
-      <c r="H1" s="298"/>
-      <c r="I1" s="298"/>
-      <c r="J1" s="298"/>
-      <c r="K1" s="298"/>
-      <c r="L1" s="298"/>
-      <c r="M1" s="298"/>
-      <c r="N1" s="298"/>
-      <c r="O1" s="299" t="s">
+      <c r="E1" s="297"/>
+      <c r="F1" s="297"/>
+      <c r="G1" s="297"/>
+      <c r="H1" s="297"/>
+      <c r="I1" s="297"/>
+      <c r="J1" s="297"/>
+      <c r="K1" s="297"/>
+      <c r="L1" s="297"/>
+      <c r="M1" s="297"/>
+      <c r="N1" s="297"/>
+      <c r="O1" s="298" t="s">
         <v>4</v>
       </c>
-      <c r="P1" s="298"/>
-      <c r="Q1" s="298"/>
-      <c r="R1" s="298"/>
-      <c r="S1" s="298"/>
-      <c r="T1" s="298"/>
-      <c r="U1" s="298"/>
-      <c r="V1" s="298"/>
-      <c r="W1" s="298"/>
-      <c r="X1" s="298"/>
-      <c r="Y1" s="298"/>
-      <c r="Z1" s="298"/>
-      <c r="AA1" s="300" t="s">
+      <c r="P1" s="297"/>
+      <c r="Q1" s="297"/>
+      <c r="R1" s="297"/>
+      <c r="S1" s="297"/>
+      <c r="T1" s="297"/>
+      <c r="U1" s="297"/>
+      <c r="V1" s="297"/>
+      <c r="W1" s="297"/>
+      <c r="X1" s="297"/>
+      <c r="Y1" s="297"/>
+      <c r="Z1" s="297"/>
+      <c r="AA1" s="299" t="s">
         <v>5</v>
       </c>
-      <c r="AB1" s="298"/>
-      <c r="AC1" s="298"/>
-      <c r="AD1" s="298"/>
-      <c r="AE1" s="298"/>
-      <c r="AF1" s="298"/>
-      <c r="AG1" s="298"/>
-      <c r="AH1" s="298"/>
-      <c r="AI1" s="298"/>
-      <c r="AJ1" s="298"/>
-      <c r="AK1" s="298"/>
-      <c r="AL1" s="212" t="s">
+      <c r="AB1" s="297"/>
+      <c r="AC1" s="297"/>
+      <c r="AD1" s="297"/>
+      <c r="AE1" s="297"/>
+      <c r="AF1" s="297"/>
+      <c r="AG1" s="297"/>
+      <c r="AH1" s="297"/>
+      <c r="AI1" s="297"/>
+      <c r="AJ1" s="297"/>
+      <c r="AK1" s="297"/>
+      <c r="AL1" s="253" t="s">
         <v>6</v>
       </c>
-      <c r="AM1" s="213"/>
-      <c r="AN1" s="213"/>
-      <c r="AO1" s="213"/>
-      <c r="AP1" s="213"/>
-      <c r="AQ1" s="213"/>
-      <c r="AR1" s="214"/>
+      <c r="AM1" s="254"/>
+      <c r="AN1" s="254"/>
+      <c r="AO1" s="254"/>
+      <c r="AP1" s="254"/>
+      <c r="AQ1" s="254"/>
+      <c r="AR1" s="255"/>
       <c r="AS1" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:45" ht="60" x14ac:dyDescent="0.25">
-      <c r="A2" s="296"/>
-      <c r="B2" s="206"/>
-      <c r="C2" s="206"/>
+      <c r="A2" s="295"/>
+      <c r="B2" s="265"/>
+      <c r="C2" s="265"/>
       <c r="D2" s="156" t="s">
         <v>8</v>
       </c>
@@ -36501,55 +36595,55 @@
       </c>
       <c r="B3" s="122"/>
       <c r="C3" s="122"/>
-      <c r="D3" s="291" t="s">
+      <c r="D3" s="290" t="s">
         <v>1283</v>
       </c>
-      <c r="E3" s="291"/>
-      <c r="F3" s="291"/>
-      <c r="G3" s="291"/>
-      <c r="H3" s="291"/>
-      <c r="I3" s="291"/>
-      <c r="J3" s="291"/>
-      <c r="K3" s="291"/>
-      <c r="L3" s="291"/>
-      <c r="M3" s="291"/>
-      <c r="N3" s="291"/>
-      <c r="O3" s="284" t="s">
+      <c r="E3" s="290"/>
+      <c r="F3" s="290"/>
+      <c r="G3" s="290"/>
+      <c r="H3" s="290"/>
+      <c r="I3" s="290"/>
+      <c r="J3" s="290"/>
+      <c r="K3" s="290"/>
+      <c r="L3" s="290"/>
+      <c r="M3" s="290"/>
+      <c r="N3" s="290"/>
+      <c r="O3" s="283" t="s">
         <v>1283</v>
       </c>
-      <c r="P3" s="284"/>
-      <c r="Q3" s="284"/>
-      <c r="R3" s="284"/>
-      <c r="S3" s="284"/>
-      <c r="T3" s="284"/>
-      <c r="U3" s="284"/>
-      <c r="V3" s="284"/>
-      <c r="W3" s="284"/>
-      <c r="X3" s="284"/>
-      <c r="Y3" s="284"/>
-      <c r="Z3" s="284"/>
-      <c r="AA3" s="291" t="s">
+      <c r="P3" s="283"/>
+      <c r="Q3" s="283"/>
+      <c r="R3" s="283"/>
+      <c r="S3" s="283"/>
+      <c r="T3" s="283"/>
+      <c r="U3" s="283"/>
+      <c r="V3" s="283"/>
+      <c r="W3" s="283"/>
+      <c r="X3" s="283"/>
+      <c r="Y3" s="283"/>
+      <c r="Z3" s="283"/>
+      <c r="AA3" s="290" t="s">
         <v>1283</v>
       </c>
-      <c r="AB3" s="291"/>
-      <c r="AC3" s="291"/>
-      <c r="AD3" s="291"/>
-      <c r="AE3" s="291"/>
-      <c r="AF3" s="291"/>
-      <c r="AG3" s="291"/>
-      <c r="AH3" s="291"/>
-      <c r="AI3" s="291"/>
-      <c r="AJ3" s="291"/>
-      <c r="AK3" s="291"/>
-      <c r="AL3" s="292" t="s">
+      <c r="AB3" s="290"/>
+      <c r="AC3" s="290"/>
+      <c r="AD3" s="290"/>
+      <c r="AE3" s="290"/>
+      <c r="AF3" s="290"/>
+      <c r="AG3" s="290"/>
+      <c r="AH3" s="290"/>
+      <c r="AI3" s="290"/>
+      <c r="AJ3" s="290"/>
+      <c r="AK3" s="290"/>
+      <c r="AL3" s="291" t="s">
         <v>1283</v>
       </c>
-      <c r="AM3" s="293"/>
-      <c r="AN3" s="293"/>
-      <c r="AO3" s="293"/>
-      <c r="AP3" s="293"/>
-      <c r="AQ3" s="293"/>
-      <c r="AR3" s="294"/>
+      <c r="AM3" s="292"/>
+      <c r="AN3" s="292"/>
+      <c r="AO3" s="292"/>
+      <c r="AP3" s="292"/>
+      <c r="AQ3" s="292"/>
+      <c r="AR3" s="293"/>
       <c r="AS3" s="157"/>
     </row>
     <row r="4" spans="1:45" s="116" customFormat="1" ht="39" x14ac:dyDescent="0.25">
@@ -37125,55 +37219,55 @@
       </c>
       <c r="B11" s="122"/>
       <c r="C11" s="122"/>
-      <c r="D11" s="291" t="s">
+      <c r="D11" s="290" t="s">
         <v>1315</v>
       </c>
-      <c r="E11" s="291"/>
-      <c r="F11" s="291"/>
-      <c r="G11" s="291"/>
-      <c r="H11" s="291"/>
-      <c r="I11" s="291"/>
-      <c r="J11" s="291"/>
-      <c r="K11" s="291"/>
-      <c r="L11" s="291"/>
-      <c r="M11" s="291"/>
-      <c r="N11" s="291"/>
-      <c r="O11" s="284" t="s">
+      <c r="E11" s="290"/>
+      <c r="F11" s="290"/>
+      <c r="G11" s="290"/>
+      <c r="H11" s="290"/>
+      <c r="I11" s="290"/>
+      <c r="J11" s="290"/>
+      <c r="K11" s="290"/>
+      <c r="L11" s="290"/>
+      <c r="M11" s="290"/>
+      <c r="N11" s="290"/>
+      <c r="O11" s="283" t="s">
         <v>1315</v>
       </c>
-      <c r="P11" s="284"/>
-      <c r="Q11" s="284"/>
-      <c r="R11" s="284"/>
-      <c r="S11" s="284"/>
-      <c r="T11" s="284"/>
-      <c r="U11" s="284"/>
-      <c r="V11" s="284"/>
-      <c r="W11" s="284"/>
-      <c r="X11" s="284"/>
-      <c r="Y11" s="284"/>
-      <c r="Z11" s="284"/>
-      <c r="AA11" s="291" t="s">
+      <c r="P11" s="283"/>
+      <c r="Q11" s="283"/>
+      <c r="R11" s="283"/>
+      <c r="S11" s="283"/>
+      <c r="T11" s="283"/>
+      <c r="U11" s="283"/>
+      <c r="V11" s="283"/>
+      <c r="W11" s="283"/>
+      <c r="X11" s="283"/>
+      <c r="Y11" s="283"/>
+      <c r="Z11" s="283"/>
+      <c r="AA11" s="290" t="s">
         <v>1315</v>
       </c>
-      <c r="AB11" s="291"/>
-      <c r="AC11" s="291"/>
-      <c r="AD11" s="291"/>
-      <c r="AE11" s="291"/>
-      <c r="AF11" s="291"/>
-      <c r="AG11" s="291"/>
-      <c r="AH11" s="291"/>
-      <c r="AI11" s="291"/>
-      <c r="AJ11" s="291"/>
-      <c r="AK11" s="291"/>
-      <c r="AL11" s="292" t="s">
+      <c r="AB11" s="290"/>
+      <c r="AC11" s="290"/>
+      <c r="AD11" s="290"/>
+      <c r="AE11" s="290"/>
+      <c r="AF11" s="290"/>
+      <c r="AG11" s="290"/>
+      <c r="AH11" s="290"/>
+      <c r="AI11" s="290"/>
+      <c r="AJ11" s="290"/>
+      <c r="AK11" s="290"/>
+      <c r="AL11" s="291" t="s">
         <v>1315</v>
       </c>
-      <c r="AM11" s="293"/>
-      <c r="AN11" s="293"/>
-      <c r="AO11" s="293"/>
-      <c r="AP11" s="293"/>
-      <c r="AQ11" s="293"/>
-      <c r="AR11" s="294"/>
+      <c r="AM11" s="292"/>
+      <c r="AN11" s="292"/>
+      <c r="AO11" s="292"/>
+      <c r="AP11" s="292"/>
+      <c r="AQ11" s="292"/>
+      <c r="AR11" s="293"/>
       <c r="AS11" s="157"/>
     </row>
     <row r="12" spans="1:45" s="116" customFormat="1" ht="39" x14ac:dyDescent="0.25">
@@ -40653,7 +40747,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:44" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="295" t="s">
+      <c r="A1" s="294" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="301" t="s">
@@ -40662,60 +40756,60 @@
       <c r="C1" s="301" t="s">
         <v>1432</v>
       </c>
-      <c r="D1" s="297" t="s">
+      <c r="D1" s="296" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="298"/>
-      <c r="F1" s="298"/>
-      <c r="G1" s="298"/>
-      <c r="H1" s="298"/>
-      <c r="I1" s="298"/>
-      <c r="J1" s="298"/>
-      <c r="K1" s="298"/>
-      <c r="L1" s="298"/>
-      <c r="M1" s="298"/>
-      <c r="N1" s="299" t="s">
+      <c r="E1" s="297"/>
+      <c r="F1" s="297"/>
+      <c r="G1" s="297"/>
+      <c r="H1" s="297"/>
+      <c r="I1" s="297"/>
+      <c r="J1" s="297"/>
+      <c r="K1" s="297"/>
+      <c r="L1" s="297"/>
+      <c r="M1" s="297"/>
+      <c r="N1" s="298" t="s">
         <v>4</v>
       </c>
-      <c r="O1" s="298"/>
-      <c r="P1" s="298"/>
-      <c r="Q1" s="298"/>
-      <c r="R1" s="298"/>
-      <c r="S1" s="298"/>
-      <c r="T1" s="298"/>
-      <c r="U1" s="298"/>
-      <c r="V1" s="298"/>
-      <c r="W1" s="298"/>
-      <c r="X1" s="298"/>
-      <c r="Y1" s="298"/>
-      <c r="Z1" s="300" t="s">
+      <c r="O1" s="297"/>
+      <c r="P1" s="297"/>
+      <c r="Q1" s="297"/>
+      <c r="R1" s="297"/>
+      <c r="S1" s="297"/>
+      <c r="T1" s="297"/>
+      <c r="U1" s="297"/>
+      <c r="V1" s="297"/>
+      <c r="W1" s="297"/>
+      <c r="X1" s="297"/>
+      <c r="Y1" s="297"/>
+      <c r="Z1" s="299" t="s">
         <v>5</v>
       </c>
-      <c r="AA1" s="298"/>
-      <c r="AB1" s="298"/>
-      <c r="AC1" s="298"/>
-      <c r="AD1" s="298"/>
-      <c r="AE1" s="298"/>
-      <c r="AF1" s="298"/>
-      <c r="AG1" s="298"/>
-      <c r="AH1" s="298"/>
-      <c r="AI1" s="298"/>
-      <c r="AJ1" s="298"/>
-      <c r="AK1" s="212" t="s">
+      <c r="AA1" s="297"/>
+      <c r="AB1" s="297"/>
+      <c r="AC1" s="297"/>
+      <c r="AD1" s="297"/>
+      <c r="AE1" s="297"/>
+      <c r="AF1" s="297"/>
+      <c r="AG1" s="297"/>
+      <c r="AH1" s="297"/>
+      <c r="AI1" s="297"/>
+      <c r="AJ1" s="297"/>
+      <c r="AK1" s="253" t="s">
         <v>6</v>
       </c>
-      <c r="AL1" s="213"/>
-      <c r="AM1" s="213"/>
-      <c r="AN1" s="213"/>
-      <c r="AO1" s="213"/>
-      <c r="AP1" s="213"/>
-      <c r="AQ1" s="214"/>
+      <c r="AL1" s="254"/>
+      <c r="AM1" s="254"/>
+      <c r="AN1" s="254"/>
+      <c r="AO1" s="254"/>
+      <c r="AP1" s="254"/>
+      <c r="AQ1" s="255"/>
       <c r="AR1" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:44" ht="60" x14ac:dyDescent="0.25">
-      <c r="A2" s="296"/>
+      <c r="A2" s="295"/>
       <c r="B2" s="302"/>
       <c r="C2" s="302"/>
       <c r="D2" s="156" t="s">
@@ -40849,54 +40943,54 @@
       </c>
       <c r="B3" s="122"/>
       <c r="C3" s="122"/>
-      <c r="D3" s="303" t="s">
+      <c r="D3" s="300" t="s">
         <v>1433</v>
       </c>
-      <c r="E3" s="303"/>
-      <c r="F3" s="303"/>
-      <c r="G3" s="303"/>
-      <c r="H3" s="303"/>
-      <c r="I3" s="303"/>
-      <c r="J3" s="303"/>
-      <c r="K3" s="303"/>
-      <c r="L3" s="303"/>
-      <c r="M3" s="303"/>
-      <c r="N3" s="303" t="s">
+      <c r="E3" s="300"/>
+      <c r="F3" s="300"/>
+      <c r="G3" s="300"/>
+      <c r="H3" s="300"/>
+      <c r="I3" s="300"/>
+      <c r="J3" s="300"/>
+      <c r="K3" s="300"/>
+      <c r="L3" s="300"/>
+      <c r="M3" s="300"/>
+      <c r="N3" s="300" t="s">
         <v>1433</v>
       </c>
-      <c r="O3" s="303"/>
-      <c r="P3" s="303"/>
-      <c r="Q3" s="303"/>
-      <c r="R3" s="303"/>
-      <c r="S3" s="303"/>
-      <c r="T3" s="303"/>
-      <c r="U3" s="303"/>
-      <c r="V3" s="303"/>
-      <c r="W3" s="303"/>
-      <c r="X3" s="303"/>
-      <c r="Y3" s="303"/>
-      <c r="Z3" s="303" t="s">
+      <c r="O3" s="300"/>
+      <c r="P3" s="300"/>
+      <c r="Q3" s="300"/>
+      <c r="R3" s="300"/>
+      <c r="S3" s="300"/>
+      <c r="T3" s="300"/>
+      <c r="U3" s="300"/>
+      <c r="V3" s="300"/>
+      <c r="W3" s="300"/>
+      <c r="X3" s="300"/>
+      <c r="Y3" s="300"/>
+      <c r="Z3" s="300" t="s">
         <v>1433</v>
       </c>
-      <c r="AA3" s="303"/>
-      <c r="AB3" s="303"/>
-      <c r="AC3" s="303"/>
-      <c r="AD3" s="303"/>
-      <c r="AE3" s="303"/>
-      <c r="AF3" s="303"/>
-      <c r="AG3" s="303"/>
-      <c r="AH3" s="303"/>
-      <c r="AI3" s="303"/>
-      <c r="AJ3" s="303"/>
-      <c r="AK3" s="280" t="s">
+      <c r="AA3" s="300"/>
+      <c r="AB3" s="300"/>
+      <c r="AC3" s="300"/>
+      <c r="AD3" s="300"/>
+      <c r="AE3" s="300"/>
+      <c r="AF3" s="300"/>
+      <c r="AG3" s="300"/>
+      <c r="AH3" s="300"/>
+      <c r="AI3" s="300"/>
+      <c r="AJ3" s="300"/>
+      <c r="AK3" s="279" t="s">
         <v>1433</v>
       </c>
-      <c r="AL3" s="281"/>
-      <c r="AM3" s="281"/>
-      <c r="AN3" s="281"/>
-      <c r="AO3" s="281"/>
-      <c r="AP3" s="281"/>
-      <c r="AQ3" s="282"/>
+      <c r="AL3" s="280"/>
+      <c r="AM3" s="280"/>
+      <c r="AN3" s="280"/>
+      <c r="AO3" s="280"/>
+      <c r="AP3" s="280"/>
+      <c r="AQ3" s="281"/>
       <c r="AR3" s="165"/>
     </row>
     <row r="4" spans="1:44" s="116" customFormat="1" ht="39" x14ac:dyDescent="0.25">
@@ -41055,54 +41149,54 @@
       </c>
       <c r="B6" s="122"/>
       <c r="C6" s="122"/>
-      <c r="D6" s="283" t="s">
+      <c r="D6" s="282" t="s">
         <v>1443</v>
       </c>
-      <c r="E6" s="283"/>
-      <c r="F6" s="283"/>
-      <c r="G6" s="283"/>
-      <c r="H6" s="283"/>
-      <c r="I6" s="283"/>
-      <c r="J6" s="283"/>
-      <c r="K6" s="283"/>
-      <c r="L6" s="283"/>
-      <c r="M6" s="283"/>
-      <c r="N6" s="284" t="s">
+      <c r="E6" s="282"/>
+      <c r="F6" s="282"/>
+      <c r="G6" s="282"/>
+      <c r="H6" s="282"/>
+      <c r="I6" s="282"/>
+      <c r="J6" s="282"/>
+      <c r="K6" s="282"/>
+      <c r="L6" s="282"/>
+      <c r="M6" s="282"/>
+      <c r="N6" s="283" t="s">
         <v>1443</v>
       </c>
-      <c r="O6" s="284"/>
-      <c r="P6" s="284"/>
-      <c r="Q6" s="284"/>
-      <c r="R6" s="284"/>
-      <c r="S6" s="284"/>
-      <c r="T6" s="284"/>
-      <c r="U6" s="284"/>
-      <c r="V6" s="284"/>
-      <c r="W6" s="284"/>
-      <c r="X6" s="284"/>
-      <c r="Y6" s="284"/>
-      <c r="Z6" s="283" t="s">
+      <c r="O6" s="283"/>
+      <c r="P6" s="283"/>
+      <c r="Q6" s="283"/>
+      <c r="R6" s="283"/>
+      <c r="S6" s="283"/>
+      <c r="T6" s="283"/>
+      <c r="U6" s="283"/>
+      <c r="V6" s="283"/>
+      <c r="W6" s="283"/>
+      <c r="X6" s="283"/>
+      <c r="Y6" s="283"/>
+      <c r="Z6" s="282" t="s">
         <v>1443</v>
       </c>
-      <c r="AA6" s="283"/>
-      <c r="AB6" s="283"/>
-      <c r="AC6" s="283"/>
-      <c r="AD6" s="283"/>
-      <c r="AE6" s="283"/>
-      <c r="AF6" s="283"/>
-      <c r="AG6" s="283"/>
-      <c r="AH6" s="283"/>
-      <c r="AI6" s="283"/>
-      <c r="AJ6" s="283"/>
-      <c r="AK6" s="285" t="s">
+      <c r="AA6" s="282"/>
+      <c r="AB6" s="282"/>
+      <c r="AC6" s="282"/>
+      <c r="AD6" s="282"/>
+      <c r="AE6" s="282"/>
+      <c r="AF6" s="282"/>
+      <c r="AG6" s="282"/>
+      <c r="AH6" s="282"/>
+      <c r="AI6" s="282"/>
+      <c r="AJ6" s="282"/>
+      <c r="AK6" s="284" t="s">
         <v>1443</v>
       </c>
-      <c r="AL6" s="286"/>
-      <c r="AM6" s="286"/>
-      <c r="AN6" s="286"/>
-      <c r="AO6" s="286"/>
-      <c r="AP6" s="286"/>
-      <c r="AQ6" s="287"/>
+      <c r="AL6" s="285"/>
+      <c r="AM6" s="285"/>
+      <c r="AN6" s="285"/>
+      <c r="AO6" s="285"/>
+      <c r="AP6" s="285"/>
+      <c r="AQ6" s="286"/>
       <c r="AR6" s="166"/>
     </row>
     <row r="7" spans="1:44" s="116" customFormat="1" ht="39" x14ac:dyDescent="0.25">
@@ -47392,54 +47486,54 @@
       </c>
       <c r="B80" s="122"/>
       <c r="C80" s="122"/>
-      <c r="D80" s="303" t="s">
+      <c r="D80" s="300" t="s">
         <v>1607</v>
       </c>
-      <c r="E80" s="303"/>
-      <c r="F80" s="303"/>
-      <c r="G80" s="303"/>
-      <c r="H80" s="303"/>
-      <c r="I80" s="303"/>
-      <c r="J80" s="303"/>
-      <c r="K80" s="303"/>
-      <c r="L80" s="303"/>
-      <c r="M80" s="303"/>
-      <c r="N80" s="303" t="s">
+      <c r="E80" s="300"/>
+      <c r="F80" s="300"/>
+      <c r="G80" s="300"/>
+      <c r="H80" s="300"/>
+      <c r="I80" s="300"/>
+      <c r="J80" s="300"/>
+      <c r="K80" s="300"/>
+      <c r="L80" s="300"/>
+      <c r="M80" s="300"/>
+      <c r="N80" s="300" t="s">
         <v>1607</v>
       </c>
-      <c r="O80" s="303"/>
-      <c r="P80" s="303"/>
-      <c r="Q80" s="303"/>
-      <c r="R80" s="303"/>
-      <c r="S80" s="303"/>
-      <c r="T80" s="303"/>
-      <c r="U80" s="303"/>
-      <c r="V80" s="303"/>
-      <c r="W80" s="303"/>
-      <c r="X80" s="303"/>
-      <c r="Y80" s="303"/>
-      <c r="Z80" s="303" t="s">
+      <c r="O80" s="300"/>
+      <c r="P80" s="300"/>
+      <c r="Q80" s="300"/>
+      <c r="R80" s="300"/>
+      <c r="S80" s="300"/>
+      <c r="T80" s="300"/>
+      <c r="U80" s="300"/>
+      <c r="V80" s="300"/>
+      <c r="W80" s="300"/>
+      <c r="X80" s="300"/>
+      <c r="Y80" s="300"/>
+      <c r="Z80" s="300" t="s">
         <v>1607</v>
       </c>
-      <c r="AA80" s="303"/>
-      <c r="AB80" s="303"/>
-      <c r="AC80" s="303"/>
-      <c r="AD80" s="303"/>
-      <c r="AE80" s="303"/>
-      <c r="AF80" s="303"/>
-      <c r="AG80" s="303"/>
-      <c r="AH80" s="303"/>
-      <c r="AI80" s="303"/>
-      <c r="AJ80" s="303"/>
-      <c r="AK80" s="280" t="s">
+      <c r="AA80" s="300"/>
+      <c r="AB80" s="300"/>
+      <c r="AC80" s="300"/>
+      <c r="AD80" s="300"/>
+      <c r="AE80" s="300"/>
+      <c r="AF80" s="300"/>
+      <c r="AG80" s="300"/>
+      <c r="AH80" s="300"/>
+      <c r="AI80" s="300"/>
+      <c r="AJ80" s="300"/>
+      <c r="AK80" s="279" t="s">
         <v>1607</v>
       </c>
-      <c r="AL80" s="281"/>
-      <c r="AM80" s="281"/>
-      <c r="AN80" s="281"/>
-      <c r="AO80" s="281"/>
-      <c r="AP80" s="281"/>
-      <c r="AQ80" s="282"/>
+      <c r="AL80" s="280"/>
+      <c r="AM80" s="280"/>
+      <c r="AN80" s="280"/>
+      <c r="AO80" s="280"/>
+      <c r="AP80" s="280"/>
+      <c r="AQ80" s="281"/>
       <c r="AR80" s="165"/>
     </row>
     <row r="81" spans="1:44" s="27" customFormat="1" ht="39" x14ac:dyDescent="0.25">
@@ -52144,6 +52238,11 @@
   </sheetData>
   <autoFilter ref="A2:AR91"/>
   <mergeCells count="19">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:M1"/>
+    <mergeCell ref="N1:Y1"/>
     <mergeCell ref="D80:M80"/>
     <mergeCell ref="N80:Y80"/>
     <mergeCell ref="Z80:AJ80"/>
@@ -52158,11 +52257,6 @@
     <mergeCell ref="Z6:AJ6"/>
     <mergeCell ref="AK6:AQ6"/>
     <mergeCell ref="Z1:AJ1"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:M1"/>
-    <mergeCell ref="N1:Y1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -52228,71 +52322,71 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:44" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="203" t="s">
+      <c r="A1" s="262" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="304" t="s">
+      <c r="B1" s="306" t="s">
         <v>1797</v>
       </c>
-      <c r="C1" s="304" t="s">
+      <c r="C1" s="306" t="s">
         <v>1796</v>
       </c>
-      <c r="D1" s="207" t="s">
+      <c r="D1" s="266" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="208"/>
-      <c r="F1" s="208"/>
-      <c r="G1" s="208"/>
-      <c r="H1" s="208"/>
-      <c r="I1" s="208"/>
-      <c r="J1" s="208"/>
-      <c r="K1" s="208"/>
-      <c r="L1" s="208"/>
-      <c r="M1" s="209"/>
-      <c r="N1" s="210" t="s">
+      <c r="E1" s="267"/>
+      <c r="F1" s="267"/>
+      <c r="G1" s="267"/>
+      <c r="H1" s="267"/>
+      <c r="I1" s="267"/>
+      <c r="J1" s="267"/>
+      <c r="K1" s="267"/>
+      <c r="L1" s="267"/>
+      <c r="M1" s="268"/>
+      <c r="N1" s="269" t="s">
         <v>4</v>
       </c>
-      <c r="O1" s="208"/>
-      <c r="P1" s="208"/>
-      <c r="Q1" s="208"/>
-      <c r="R1" s="208"/>
-      <c r="S1" s="208"/>
-      <c r="T1" s="208"/>
-      <c r="U1" s="208"/>
-      <c r="V1" s="208"/>
-      <c r="W1" s="208"/>
-      <c r="X1" s="208"/>
-      <c r="Y1" s="209"/>
-      <c r="Z1" s="211" t="s">
+      <c r="O1" s="267"/>
+      <c r="P1" s="267"/>
+      <c r="Q1" s="267"/>
+      <c r="R1" s="267"/>
+      <c r="S1" s="267"/>
+      <c r="T1" s="267"/>
+      <c r="U1" s="267"/>
+      <c r="V1" s="267"/>
+      <c r="W1" s="267"/>
+      <c r="X1" s="267"/>
+      <c r="Y1" s="268"/>
+      <c r="Z1" s="270" t="s">
         <v>5</v>
       </c>
-      <c r="AA1" s="208"/>
-      <c r="AB1" s="208"/>
-      <c r="AC1" s="208"/>
-      <c r="AD1" s="208"/>
-      <c r="AE1" s="208"/>
-      <c r="AF1" s="208"/>
-      <c r="AG1" s="208"/>
-      <c r="AH1" s="208"/>
-      <c r="AI1" s="208"/>
-      <c r="AJ1" s="209"/>
-      <c r="AK1" s="212" t="s">
+      <c r="AA1" s="267"/>
+      <c r="AB1" s="267"/>
+      <c r="AC1" s="267"/>
+      <c r="AD1" s="267"/>
+      <c r="AE1" s="267"/>
+      <c r="AF1" s="267"/>
+      <c r="AG1" s="267"/>
+      <c r="AH1" s="267"/>
+      <c r="AI1" s="267"/>
+      <c r="AJ1" s="268"/>
+      <c r="AK1" s="253" t="s">
         <v>6</v>
       </c>
-      <c r="AL1" s="213"/>
-      <c r="AM1" s="213"/>
-      <c r="AN1" s="213"/>
-      <c r="AO1" s="213"/>
-      <c r="AP1" s="213"/>
-      <c r="AQ1" s="214"/>
+      <c r="AL1" s="254"/>
+      <c r="AM1" s="254"/>
+      <c r="AN1" s="254"/>
+      <c r="AO1" s="254"/>
+      <c r="AP1" s="254"/>
+      <c r="AQ1" s="255"/>
       <c r="AR1" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:44" ht="60" x14ac:dyDescent="0.25">
-      <c r="A2" s="305"/>
-      <c r="B2" s="305"/>
-      <c r="C2" s="305"/>
+      <c r="A2" s="307"/>
+      <c r="B2" s="307"/>
+      <c r="C2" s="307"/>
       <c r="D2" s="156" t="s">
         <v>8</v>
       </c>
@@ -52447,29 +52541,29 @@
       <c r="V3" s="172"/>
       <c r="W3" s="172"/>
       <c r="X3" s="172"/>
-      <c r="Y3" s="291" t="s">
+      <c r="Y3" s="290" t="s">
         <v>1795</v>
       </c>
-      <c r="Z3" s="298"/>
-      <c r="AA3" s="298"/>
-      <c r="AB3" s="298"/>
-      <c r="AC3" s="298"/>
-      <c r="AD3" s="298"/>
-      <c r="AE3" s="298"/>
-      <c r="AF3" s="298"/>
-      <c r="AG3" s="298"/>
-      <c r="AH3" s="298"/>
-      <c r="AI3" s="298"/>
+      <c r="Z3" s="297"/>
+      <c r="AA3" s="297"/>
+      <c r="AB3" s="297"/>
+      <c r="AC3" s="297"/>
+      <c r="AD3" s="297"/>
+      <c r="AE3" s="297"/>
+      <c r="AF3" s="297"/>
+      <c r="AG3" s="297"/>
+      <c r="AH3" s="297"/>
+      <c r="AI3" s="297"/>
       <c r="AJ3" s="157"/>
-      <c r="AK3" s="306" t="s">
+      <c r="AK3" s="303" t="s">
         <v>1794</v>
       </c>
-      <c r="AL3" s="307"/>
-      <c r="AM3" s="307"/>
-      <c r="AN3" s="307"/>
-      <c r="AO3" s="307"/>
-      <c r="AP3" s="307"/>
-      <c r="AQ3" s="308"/>
+      <c r="AL3" s="304"/>
+      <c r="AM3" s="304"/>
+      <c r="AN3" s="304"/>
+      <c r="AO3" s="304"/>
+      <c r="AP3" s="304"/>
+      <c r="AQ3" s="305"/>
       <c r="AR3" s="11"/>
     </row>
     <row r="4" spans="1:44" s="116" customFormat="1" ht="39" x14ac:dyDescent="0.25">
@@ -53184,42 +53278,42 @@
       <c r="K13" s="171"/>
       <c r="L13" s="171"/>
       <c r="M13" s="171"/>
-      <c r="N13" s="284" t="s">
+      <c r="N13" s="283" t="s">
         <v>1778</v>
       </c>
-      <c r="O13" s="298"/>
-      <c r="P13" s="298"/>
-      <c r="Q13" s="298"/>
-      <c r="R13" s="298"/>
-      <c r="S13" s="298"/>
-      <c r="T13" s="298"/>
-      <c r="U13" s="298"/>
-      <c r="V13" s="298"/>
-      <c r="W13" s="298"/>
-      <c r="X13" s="298"/>
-      <c r="Y13" s="298"/>
-      <c r="Z13" s="291" t="s">
+      <c r="O13" s="297"/>
+      <c r="P13" s="297"/>
+      <c r="Q13" s="297"/>
+      <c r="R13" s="297"/>
+      <c r="S13" s="297"/>
+      <c r="T13" s="297"/>
+      <c r="U13" s="297"/>
+      <c r="V13" s="297"/>
+      <c r="W13" s="297"/>
+      <c r="X13" s="297"/>
+      <c r="Y13" s="297"/>
+      <c r="Z13" s="290" t="s">
         <v>1778</v>
       </c>
-      <c r="AA13" s="291"/>
-      <c r="AB13" s="291"/>
-      <c r="AC13" s="291"/>
-      <c r="AD13" s="291"/>
-      <c r="AE13" s="291"/>
-      <c r="AF13" s="291"/>
-      <c r="AG13" s="291"/>
-      <c r="AH13" s="291"/>
-      <c r="AI13" s="291"/>
-      <c r="AJ13" s="291"/>
-      <c r="AK13" s="306" t="s">
+      <c r="AA13" s="290"/>
+      <c r="AB13" s="290"/>
+      <c r="AC13" s="290"/>
+      <c r="AD13" s="290"/>
+      <c r="AE13" s="290"/>
+      <c r="AF13" s="290"/>
+      <c r="AG13" s="290"/>
+      <c r="AH13" s="290"/>
+      <c r="AI13" s="290"/>
+      <c r="AJ13" s="290"/>
+      <c r="AK13" s="303" t="s">
         <v>1778</v>
       </c>
-      <c r="AL13" s="307"/>
-      <c r="AM13" s="307"/>
-      <c r="AN13" s="307"/>
-      <c r="AO13" s="307"/>
-      <c r="AP13" s="307"/>
-      <c r="AQ13" s="308"/>
+      <c r="AL13" s="304"/>
+      <c r="AM13" s="304"/>
+      <c r="AN13" s="304"/>
+      <c r="AO13" s="304"/>
+      <c r="AP13" s="304"/>
+      <c r="AQ13" s="305"/>
       <c r="AR13" s="52"/>
     </row>
     <row r="14" spans="1:44" s="116" customFormat="1" ht="39" x14ac:dyDescent="0.25">
@@ -56596,18 +56690,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="D1:M1"/>
+    <mergeCell ref="N1:Y1"/>
+    <mergeCell ref="Z1:AJ1"/>
+    <mergeCell ref="C1:C2"/>
     <mergeCell ref="AK1:AQ1"/>
     <mergeCell ref="AK3:AQ3"/>
     <mergeCell ref="AK13:AQ13"/>
     <mergeCell ref="Y3:AI3"/>
     <mergeCell ref="Z13:AJ13"/>
     <mergeCell ref="N13:Y13"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="D1:M1"/>
-    <mergeCell ref="N1:Y1"/>
-    <mergeCell ref="Z1:AJ1"/>
-    <mergeCell ref="C1:C2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -56620,7 +56714,7 @@
   </sheetPr>
   <dimension ref="A1:AV112"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView topLeftCell="H51" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="P6" sqref="P6"/>
     </sheetView>
   </sheetViews>
@@ -56664,69 +56758,69 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:48" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="203" t="s">
+      <c r="A1" s="262" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="304" t="s">
+      <c r="B1" s="306" t="s">
         <v>1797</v>
       </c>
-      <c r="C1" s="304" t="s">
+      <c r="C1" s="306" t="s">
         <v>1796</v>
       </c>
-      <c r="D1" s="207" t="s">
+      <c r="D1" s="266" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="208"/>
-      <c r="F1" s="208"/>
-      <c r="G1" s="208"/>
-      <c r="H1" s="208"/>
-      <c r="I1" s="208"/>
-      <c r="J1" s="208"/>
-      <c r="K1" s="208"/>
-      <c r="L1" s="208"/>
-      <c r="M1" s="209"/>
-      <c r="N1" s="210" t="s">
+      <c r="E1" s="267"/>
+      <c r="F1" s="267"/>
+      <c r="G1" s="267"/>
+      <c r="H1" s="267"/>
+      <c r="I1" s="267"/>
+      <c r="J1" s="267"/>
+      <c r="K1" s="267"/>
+      <c r="L1" s="267"/>
+      <c r="M1" s="268"/>
+      <c r="N1" s="269" t="s">
         <v>4</v>
       </c>
-      <c r="O1" s="309"/>
-      <c r="P1" s="309"/>
-      <c r="Q1" s="309"/>
-      <c r="R1" s="309"/>
-      <c r="S1" s="309"/>
-      <c r="T1" s="309"/>
-      <c r="U1" s="309"/>
-      <c r="V1" s="309"/>
-      <c r="W1" s="309"/>
-      <c r="X1" s="310"/>
-      <c r="Y1" s="211" t="s">
+      <c r="O1" s="308"/>
+      <c r="P1" s="308"/>
+      <c r="Q1" s="308"/>
+      <c r="R1" s="308"/>
+      <c r="S1" s="308"/>
+      <c r="T1" s="308"/>
+      <c r="U1" s="308"/>
+      <c r="V1" s="308"/>
+      <c r="W1" s="308"/>
+      <c r="X1" s="309"/>
+      <c r="Y1" s="270" t="s">
         <v>4</v>
       </c>
-      <c r="Z1" s="208"/>
-      <c r="AA1" s="208"/>
-      <c r="AB1" s="208"/>
-      <c r="AC1" s="208"/>
-      <c r="AD1" s="208"/>
-      <c r="AE1" s="208"/>
-      <c r="AF1" s="208"/>
-      <c r="AG1" s="208"/>
-      <c r="AH1" s="208"/>
-      <c r="AI1" s="212" t="s">
+      <c r="Z1" s="267"/>
+      <c r="AA1" s="267"/>
+      <c r="AB1" s="267"/>
+      <c r="AC1" s="267"/>
+      <c r="AD1" s="267"/>
+      <c r="AE1" s="267"/>
+      <c r="AF1" s="267"/>
+      <c r="AG1" s="267"/>
+      <c r="AH1" s="267"/>
+      <c r="AI1" s="253" t="s">
         <v>6</v>
       </c>
-      <c r="AJ1" s="213"/>
-      <c r="AK1" s="213"/>
-      <c r="AL1" s="213"/>
-      <c r="AM1" s="213"/>
-      <c r="AN1" s="213"/>
-      <c r="AO1" s="214"/>
+      <c r="AJ1" s="254"/>
+      <c r="AK1" s="254"/>
+      <c r="AL1" s="254"/>
+      <c r="AM1" s="254"/>
+      <c r="AN1" s="254"/>
+      <c r="AO1" s="255"/>
       <c r="AP1" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:48" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="305"/>
-      <c r="B2" s="305"/>
-      <c r="C2" s="305"/>
+      <c r="A2" s="307"/>
+      <c r="B2" s="307"/>
+      <c r="C2" s="307"/>
       <c r="D2" s="156" t="s">
         <v>8</v>
       </c>
@@ -56850,52 +56944,52 @@
       </c>
       <c r="B3" s="173"/>
       <c r="C3" s="173"/>
-      <c r="D3" s="291" t="s">
+      <c r="D3" s="290" t="s">
         <v>1798</v>
       </c>
-      <c r="E3" s="291"/>
-      <c r="F3" s="291"/>
-      <c r="G3" s="291"/>
-      <c r="H3" s="291"/>
-      <c r="I3" s="291"/>
-      <c r="J3" s="291"/>
-      <c r="K3" s="291"/>
-      <c r="L3" s="291"/>
-      <c r="M3" s="291"/>
-      <c r="N3" s="291" t="s">
+      <c r="E3" s="290"/>
+      <c r="F3" s="290"/>
+      <c r="G3" s="290"/>
+      <c r="H3" s="290"/>
+      <c r="I3" s="290"/>
+      <c r="J3" s="290"/>
+      <c r="K3" s="290"/>
+      <c r="L3" s="290"/>
+      <c r="M3" s="290"/>
+      <c r="N3" s="290" t="s">
         <v>1798</v>
       </c>
-      <c r="O3" s="291"/>
-      <c r="P3" s="291"/>
-      <c r="Q3" s="291"/>
-      <c r="R3" s="291"/>
-      <c r="S3" s="291"/>
-      <c r="T3" s="291"/>
-      <c r="U3" s="291"/>
-      <c r="V3" s="291"/>
-      <c r="W3" s="291"/>
-      <c r="X3" s="291"/>
-      <c r="Y3" s="291"/>
-      <c r="Z3" s="284" t="s">
+      <c r="O3" s="290"/>
+      <c r="P3" s="290"/>
+      <c r="Q3" s="290"/>
+      <c r="R3" s="290"/>
+      <c r="S3" s="290"/>
+      <c r="T3" s="290"/>
+      <c r="U3" s="290"/>
+      <c r="V3" s="290"/>
+      <c r="W3" s="290"/>
+      <c r="X3" s="290"/>
+      <c r="Y3" s="290"/>
+      <c r="Z3" s="283" t="s">
         <v>1798</v>
       </c>
-      <c r="AA3" s="284"/>
-      <c r="AB3" s="284"/>
-      <c r="AC3" s="284"/>
-      <c r="AD3" s="284"/>
-      <c r="AE3" s="284"/>
-      <c r="AF3" s="284"/>
-      <c r="AG3" s="284"/>
-      <c r="AH3" s="284"/>
-      <c r="AI3" s="292" t="s">
+      <c r="AA3" s="283"/>
+      <c r="AB3" s="283"/>
+      <c r="AC3" s="283"/>
+      <c r="AD3" s="283"/>
+      <c r="AE3" s="283"/>
+      <c r="AF3" s="283"/>
+      <c r="AG3" s="283"/>
+      <c r="AH3" s="283"/>
+      <c r="AI3" s="291" t="s">
         <v>1798</v>
       </c>
-      <c r="AJ3" s="293"/>
-      <c r="AK3" s="293"/>
-      <c r="AL3" s="293"/>
-      <c r="AM3" s="293"/>
-      <c r="AN3" s="293"/>
-      <c r="AO3" s="294"/>
+      <c r="AJ3" s="292"/>
+      <c r="AK3" s="292"/>
+      <c r="AL3" s="292"/>
+      <c r="AM3" s="292"/>
+      <c r="AN3" s="292"/>
+      <c r="AO3" s="293"/>
       <c r="AP3" s="171"/>
     </row>
     <row r="4" spans="1:48" s="116" customFormat="1" ht="26.25" x14ac:dyDescent="0.25">
@@ -60962,50 +61056,50 @@
       </c>
       <c r="B53" s="173"/>
       <c r="C53" s="173"/>
-      <c r="D53" s="291"/>
-      <c r="E53" s="291"/>
-      <c r="F53" s="291"/>
-      <c r="G53" s="291"/>
-      <c r="H53" s="291"/>
-      <c r="I53" s="291"/>
-      <c r="J53" s="291"/>
-      <c r="K53" s="291"/>
-      <c r="L53" s="291"/>
-      <c r="M53" s="291"/>
-      <c r="N53" s="291" t="s">
+      <c r="D53" s="290"/>
+      <c r="E53" s="290"/>
+      <c r="F53" s="290"/>
+      <c r="G53" s="290"/>
+      <c r="H53" s="290"/>
+      <c r="I53" s="290"/>
+      <c r="J53" s="290"/>
+      <c r="K53" s="290"/>
+      <c r="L53" s="290"/>
+      <c r="M53" s="290"/>
+      <c r="N53" s="290" t="s">
         <v>1932</v>
       </c>
-      <c r="O53" s="291"/>
-      <c r="P53" s="291"/>
-      <c r="Q53" s="291"/>
-      <c r="R53" s="291"/>
-      <c r="S53" s="291"/>
-      <c r="T53" s="291"/>
-      <c r="U53" s="291"/>
-      <c r="V53" s="291"/>
-      <c r="W53" s="291"/>
-      <c r="X53" s="291"/>
-      <c r="Y53" s="291"/>
-      <c r="Z53" s="284" t="s">
+      <c r="O53" s="290"/>
+      <c r="P53" s="290"/>
+      <c r="Q53" s="290"/>
+      <c r="R53" s="290"/>
+      <c r="S53" s="290"/>
+      <c r="T53" s="290"/>
+      <c r="U53" s="290"/>
+      <c r="V53" s="290"/>
+      <c r="W53" s="290"/>
+      <c r="X53" s="290"/>
+      <c r="Y53" s="290"/>
+      <c r="Z53" s="283" t="s">
         <v>1932</v>
       </c>
-      <c r="AA53" s="284"/>
-      <c r="AB53" s="284"/>
-      <c r="AC53" s="284"/>
-      <c r="AD53" s="284"/>
-      <c r="AE53" s="284"/>
-      <c r="AF53" s="284"/>
-      <c r="AG53" s="284"/>
-      <c r="AH53" s="284"/>
-      <c r="AI53" s="292" t="s">
+      <c r="AA53" s="283"/>
+      <c r="AB53" s="283"/>
+      <c r="AC53" s="283"/>
+      <c r="AD53" s="283"/>
+      <c r="AE53" s="283"/>
+      <c r="AF53" s="283"/>
+      <c r="AG53" s="283"/>
+      <c r="AH53" s="283"/>
+      <c r="AI53" s="291" t="s">
         <v>1932</v>
       </c>
-      <c r="AJ53" s="293"/>
-      <c r="AK53" s="293"/>
-      <c r="AL53" s="293"/>
-      <c r="AM53" s="293"/>
-      <c r="AN53" s="293"/>
-      <c r="AO53" s="294"/>
+      <c r="AJ53" s="292"/>
+      <c r="AK53" s="292"/>
+      <c r="AL53" s="292"/>
+      <c r="AM53" s="292"/>
+      <c r="AN53" s="292"/>
+      <c r="AO53" s="293"/>
       <c r="AP53" s="171"/>
     </row>
     <row r="54" spans="1:42" s="116" customFormat="1" ht="26.25" x14ac:dyDescent="0.25">

</xml_diff>